<commit_message>
Pablo: test cases para us 1, 2 y 3
</commit_message>
<xml_diff>
--- a/Docs/08-Prueba/Tests Cases - Modulo de Planificación.xlsx
+++ b/Docs/08-Prueba/Tests Cases - Modulo de Planificación.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="405" windowWidth="18675" windowHeight="8160" activeTab="3"/>
+    <workbookView xWindow="360" yWindow="405" windowWidth="18675" windowHeight="8160" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Reference" sheetId="27" r:id="rId1"/>
@@ -19,12 +19,11 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">US_135!$A$1:$J$1</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="124">
   <si>
     <t>Application</t>
   </si>
@@ -358,6 +357,96 @@
   </si>
   <si>
     <t>La planificación es listada y es editable.</t>
+  </si>
+  <si>
+    <t>Este Test Case tiene como objeto verificar la modificación satisfactoria de un contenido.</t>
+  </si>
+  <si>
+    <t>TC1_US2</t>
+  </si>
+  <si>
+    <t>TC2_US2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seleccionar la opción "Planificación" de uno de los contenidos mostrados. </t>
+  </si>
+  <si>
+    <t>Se muestra la página de edición de planificación, con las fechas de Inicio y Finalización, Contenidos, Criterios, Estrategias e Instrumentos de Evaluación. Además se dispone de las opciones de Guardar y Contenidos.</t>
+  </si>
+  <si>
+    <t>El usuario realiza un cambio en cualquiera de esos campos</t>
+  </si>
+  <si>
+    <t>El usuario hace click en el botón Guardar</t>
+  </si>
+  <si>
+    <t>El sistema regresa a la página de listado de contenidos.</t>
+  </si>
+  <si>
+    <t>Este Test Case tiene como objeto verificar que si el usuario vuelve a la página anterior sin guardar, los cambios no serán persistidos.</t>
+  </si>
+  <si>
+    <t>El usuario hace click en el botón Volver</t>
+  </si>
+  <si>
+    <t>El usuario realiza un cambio en la fecha de inicio, agregandole un día</t>
+  </si>
+  <si>
+    <t>El sistema muestra la página de edición y la fecha no ha sido persistida</t>
+  </si>
+  <si>
+    <t>TC3_US2</t>
+  </si>
+  <si>
+    <t>El usuario hace click en el botón Contenidos</t>
+  </si>
+  <si>
+    <t>Se muestran los contenidos asociados</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El usuario selecciona el contenido "Grupos étnicos - diversidad" </t>
+  </si>
+  <si>
+    <t>El usuario hace click en guardar</t>
+  </si>
+  <si>
+    <t>Se cierra el popup</t>
+  </si>
+  <si>
+    <t>El usuario es dirigido a la página de edición nuevamente</t>
+  </si>
+  <si>
+    <t>Este Test Case tiene como objeto verificar la no modificación de un contenido asociado si el usuario no guarda los cambios.</t>
+  </si>
+  <si>
+    <t>Este Test Case tiene como objeto verificar la modificación de un contenido asociado si el usuario guarda los cambios.</t>
+  </si>
+  <si>
+    <t>TC4_US2</t>
+  </si>
+  <si>
+    <t>El usuario hace click en Volver</t>
+  </si>
+  <si>
+    <t>Se muestran los contenidos asociados y el de "Grupos étnicos - diversidad" no está seleccionado</t>
+  </si>
+  <si>
+    <t>Se muestran los contenidos asociados y el de "Grupos étnicos - diversidad" está seleccionado.</t>
+  </si>
+  <si>
+    <t>TC4_US1</t>
+  </si>
+  <si>
+    <t>Este Test Case tiene como objeto verificar la correcta creación de una planificación y sin contenidos asignados, la cual posee una currícula aprobada.</t>
+  </si>
+  <si>
+    <t>Seleccionar la opción "Volver"</t>
+  </si>
+  <si>
+    <t>TC1_US3</t>
+  </si>
+  <si>
+    <t>TC2_US3</t>
   </si>
 </sst>
 </file>
@@ -515,12 +604,6 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -541,6 +624,12 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -891,7 +980,7 @@
   <dimension ref="A1:J38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E2" sqref="E2:F2"/>
     </sheetView>
   </sheetViews>
@@ -936,13 +1025,13 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="21.75" thickBot="1">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="9" t="s">
         <v>21</v>
       </c>
       <c r="D2" s="3">
@@ -955,14 +1044,14 @@
         <v>67</v>
       </c>
       <c r="G2" s="4"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
     </row>
     <row r="3" spans="1:10" ht="21.75" thickBot="1">
-      <c r="A3" s="8"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="12"/>
+      <c r="A3" s="6"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="10"/>
       <c r="D3" s="3">
         <v>2</v>
       </c>
@@ -973,14 +1062,14 @@
         <v>23</v>
       </c>
       <c r="G3" s="4"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
     </row>
     <row r="4" spans="1:10" ht="21.75" thickBot="1">
-      <c r="A4" s="8"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="12"/>
+      <c r="A4" s="6"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="10"/>
       <c r="D4" s="3">
         <v>3</v>
       </c>
@@ -991,14 +1080,14 @@
         <v>19</v>
       </c>
       <c r="G4" s="4"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
     </row>
     <row r="5" spans="1:10" ht="42.75" thickBot="1">
-      <c r="A5" s="8"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="12"/>
+      <c r="A5" s="6"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="10"/>
       <c r="D5" s="3">
         <v>4</v>
       </c>
@@ -1009,14 +1098,14 @@
         <v>24</v>
       </c>
       <c r="G5" s="4"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
     </row>
     <row r="6" spans="1:10" ht="21.75" thickBot="1">
-      <c r="A6" s="8"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="12"/>
+      <c r="A6" s="6"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="10"/>
       <c r="D6" s="3">
         <v>5</v>
       </c>
@@ -1027,14 +1116,14 @@
         <v>25</v>
       </c>
       <c r="G6" s="4"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
     </row>
     <row r="7" spans="1:10" ht="42.75" thickBot="1">
-      <c r="A7" s="8"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="12"/>
+      <c r="A7" s="6"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="10"/>
       <c r="D7" s="3">
         <v>6</v>
       </c>
@@ -1045,9 +1134,9 @@
         <v>27</v>
       </c>
       <c r="G7" s="4"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
     </row>
     <row r="8" spans="1:10" ht="15.75" thickBot="1">
       <c r="A8" s="1"/>
@@ -1062,13 +1151,13 @@
       <c r="J8" s="1"/>
     </row>
     <row r="9" spans="1:10" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="9" t="s">
         <v>29</v>
       </c>
       <c r="D9" s="3">
@@ -1081,14 +1170,14 @@
         <v>67</v>
       </c>
       <c r="G9" s="4"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A10" s="8"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="12"/>
+      <c r="A10" s="6"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="10"/>
       <c r="D10" s="3">
         <v>2</v>
       </c>
@@ -1099,14 +1188,14 @@
         <v>23</v>
       </c>
       <c r="G10" s="4"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
     </row>
     <row r="11" spans="1:10" ht="21.75" thickBot="1">
-      <c r="A11" s="8"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="12"/>
+      <c r="A11" s="6"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="10"/>
       <c r="D11" s="3">
         <v>3</v>
       </c>
@@ -1117,14 +1206,14 @@
         <v>19</v>
       </c>
       <c r="G11" s="4"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
     </row>
     <row r="12" spans="1:10" ht="42.75" thickBot="1">
-      <c r="A12" s="8"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="12"/>
+      <c r="A12" s="6"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="10"/>
       <c r="D12" s="3">
         <v>4</v>
       </c>
@@ -1135,14 +1224,14 @@
         <v>24</v>
       </c>
       <c r="G12" s="4"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
     </row>
     <row r="13" spans="1:10" ht="21.75" thickBot="1">
-      <c r="A13" s="8"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="12"/>
+      <c r="A13" s="6"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="10"/>
       <c r="D13" s="3">
         <v>5</v>
       </c>
@@ -1153,14 +1242,14 @@
         <v>25</v>
       </c>
       <c r="G13" s="4"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
     </row>
     <row r="14" spans="1:10" ht="42.75" thickBot="1">
-      <c r="A14" s="8"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="13"/>
+      <c r="A14" s="6"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="11"/>
       <c r="D14" s="3">
         <v>6</v>
       </c>
@@ -1171,9 +1260,9 @@
         <v>31</v>
       </c>
       <c r="G14" s="4"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
     </row>
     <row r="15" spans="1:10" ht="15.75" thickBot="1">
       <c r="A15" s="1"/>
@@ -1188,13 +1277,13 @@
       <c r="J15" s="1"/>
     </row>
     <row r="16" spans="1:10" ht="21.75" thickBot="1">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="9" t="s">
         <v>32</v>
       </c>
       <c r="D16" s="3">
@@ -1207,14 +1296,14 @@
         <v>67</v>
       </c>
       <c r="G16" s="4"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:10" ht="21.75" thickBot="1">
-      <c r="A17" s="8"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="12"/>
+      <c r="A17" s="6"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="10"/>
       <c r="D17" s="3">
         <v>2</v>
       </c>
@@ -1225,14 +1314,14 @@
         <v>23</v>
       </c>
       <c r="G17" s="4"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="8"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
     </row>
     <row r="18" spans="1:10" ht="21.75" thickBot="1">
-      <c r="A18" s="8"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="12"/>
+      <c r="A18" s="6"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="10"/>
       <c r="D18" s="3">
         <v>3</v>
       </c>
@@ -1243,14 +1332,14 @@
         <v>19</v>
       </c>
       <c r="G18" s="4"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="8"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
     </row>
     <row r="19" spans="1:10" ht="42.75" thickBot="1">
-      <c r="A19" s="8"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="12"/>
+      <c r="A19" s="6"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="10"/>
       <c r="D19" s="3">
         <v>4</v>
       </c>
@@ -1261,14 +1350,14 @@
         <v>24</v>
       </c>
       <c r="G19" s="4"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
     </row>
     <row r="20" spans="1:10" ht="32.25" thickBot="1">
-      <c r="A20" s="8"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="12"/>
+      <c r="A20" s="6"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="10"/>
       <c r="D20" s="3">
         <v>5</v>
       </c>
@@ -1279,14 +1368,14 @@
         <v>34</v>
       </c>
       <c r="G20" s="4"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="8"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
     </row>
     <row r="21" spans="1:10" ht="32.25" thickBot="1">
-      <c r="A21" s="8"/>
-      <c r="B21" s="10"/>
-      <c r="C21" s="12"/>
+      <c r="A21" s="6"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="10"/>
       <c r="D21" s="3">
         <v>6</v>
       </c>
@@ -1297,14 +1386,14 @@
         <v>35</v>
       </c>
       <c r="G21" s="4"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="8"/>
-      <c r="J21" s="8"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
     </row>
     <row r="22" spans="1:10" ht="42.75" thickBot="1">
-      <c r="A22" s="8"/>
-      <c r="B22" s="10"/>
-      <c r="C22" s="12"/>
+      <c r="A22" s="6"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="10"/>
       <c r="D22" s="3">
         <v>7</v>
       </c>
@@ -1315,9 +1404,9 @@
         <v>37</v>
       </c>
       <c r="G22" s="4"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="8"/>
-      <c r="J22" s="8"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
     </row>
     <row r="23" spans="1:10" ht="15.75" thickBot="1">
       <c r="A23" s="1"/>
@@ -1332,13 +1421,13 @@
       <c r="J23" s="1"/>
     </row>
     <row r="24" spans="1:10" ht="21.75" thickBot="1">
-      <c r="A24" s="7" t="s">
+      <c r="A24" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B24" s="9" t="s">
+      <c r="B24" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="C24" s="9" t="s">
         <v>40</v>
       </c>
       <c r="D24" s="3">
@@ -1351,14 +1440,14 @@
         <v>67</v>
       </c>
       <c r="G24" s="4"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="7"/>
-      <c r="J24" s="7"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
     </row>
     <row r="25" spans="1:10" ht="21.75" thickBot="1">
-      <c r="A25" s="8"/>
-      <c r="B25" s="10"/>
-      <c r="C25" s="12"/>
+      <c r="A25" s="6"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="10"/>
       <c r="D25" s="3">
         <v>2</v>
       </c>
@@ -1369,14 +1458,14 @@
         <v>23</v>
       </c>
       <c r="G25" s="4"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="8"/>
-      <c r="J25" s="8"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="6"/>
     </row>
     <row r="26" spans="1:10" ht="21.75" thickBot="1">
-      <c r="A26" s="8"/>
-      <c r="B26" s="10"/>
-      <c r="C26" s="12"/>
+      <c r="A26" s="6"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="10"/>
       <c r="D26" s="3">
         <v>3</v>
       </c>
@@ -1387,14 +1476,14 @@
         <v>19</v>
       </c>
       <c r="G26" s="4"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="8"/>
-      <c r="J26" s="8"/>
+      <c r="H26" s="13"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="42.75" thickBot="1">
-      <c r="A27" s="8"/>
-      <c r="B27" s="10"/>
-      <c r="C27" s="12"/>
+      <c r="A27" s="6"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="10"/>
       <c r="D27" s="3">
         <v>4</v>
       </c>
@@ -1405,14 +1494,14 @@
         <v>24</v>
       </c>
       <c r="G27" s="4"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="8"/>
-      <c r="J27" s="8"/>
+      <c r="H27" s="13"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="21.75" thickBot="1">
-      <c r="A28" s="8"/>
-      <c r="B28" s="10"/>
-      <c r="C28" s="12"/>
+      <c r="A28" s="6"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="10"/>
       <c r="D28" s="3">
         <v>5</v>
       </c>
@@ -1423,14 +1512,14 @@
         <v>25</v>
       </c>
       <c r="G28" s="4"/>
-      <c r="H28" s="6"/>
-      <c r="I28" s="8"/>
-      <c r="J28" s="8"/>
+      <c r="H28" s="13"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="6"/>
     </row>
     <row r="29" spans="1:10" ht="32.25" thickBot="1">
-      <c r="A29" s="8"/>
-      <c r="B29" s="10"/>
-      <c r="C29" s="12"/>
+      <c r="A29" s="6"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="10"/>
       <c r="D29" s="3">
         <v>6</v>
       </c>
@@ -1441,9 +1530,9 @@
         <v>39</v>
       </c>
       <c r="G29" s="4"/>
-      <c r="H29" s="6"/>
-      <c r="I29" s="8"/>
-      <c r="J29" s="8"/>
+      <c r="H29" s="13"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="6"/>
     </row>
     <row r="30" spans="1:10" ht="15.75" thickBot="1">
       <c r="A30" s="1"/>
@@ -1458,13 +1547,13 @@
       <c r="J30" s="1"/>
     </row>
     <row r="31" spans="1:10" ht="21.75" thickBot="1">
-      <c r="A31" s="7" t="s">
+      <c r="A31" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B31" s="9" t="s">
+      <c r="B31" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="C31" s="11" t="s">
+      <c r="C31" s="9" t="s">
         <v>41</v>
       </c>
       <c r="D31" s="3">
@@ -1477,14 +1566,14 @@
         <v>67</v>
       </c>
       <c r="G31" s="4"/>
-      <c r="H31" s="5"/>
-      <c r="I31" s="7"/>
-      <c r="J31" s="7"/>
+      <c r="H31" s="12"/>
+      <c r="I31" s="5"/>
+      <c r="J31" s="5"/>
     </row>
     <row r="32" spans="1:10" ht="21.75" thickBot="1">
-      <c r="A32" s="8"/>
-      <c r="B32" s="10"/>
-      <c r="C32" s="12"/>
+      <c r="A32" s="6"/>
+      <c r="B32" s="8"/>
+      <c r="C32" s="10"/>
       <c r="D32" s="3">
         <v>2</v>
       </c>
@@ -1495,14 +1584,14 @@
         <v>23</v>
       </c>
       <c r="G32" s="4"/>
-      <c r="H32" s="6"/>
-      <c r="I32" s="8"/>
-      <c r="J32" s="8"/>
+      <c r="H32" s="13"/>
+      <c r="I32" s="6"/>
+      <c r="J32" s="6"/>
     </row>
     <row r="33" spans="1:10" ht="21.75" thickBot="1">
-      <c r="A33" s="8"/>
-      <c r="B33" s="10"/>
-      <c r="C33" s="12"/>
+      <c r="A33" s="6"/>
+      <c r="B33" s="8"/>
+      <c r="C33" s="10"/>
       <c r="D33" s="3">
         <v>3</v>
       </c>
@@ -1513,14 +1602,14 @@
         <v>19</v>
       </c>
       <c r="G33" s="4"/>
-      <c r="H33" s="6"/>
-      <c r="I33" s="8"/>
-      <c r="J33" s="8"/>
+      <c r="H33" s="13"/>
+      <c r="I33" s="6"/>
+      <c r="J33" s="6"/>
     </row>
     <row r="34" spans="1:10" ht="42.75" thickBot="1">
-      <c r="A34" s="8"/>
-      <c r="B34" s="10"/>
-      <c r="C34" s="12"/>
+      <c r="A34" s="6"/>
+      <c r="B34" s="8"/>
+      <c r="C34" s="10"/>
       <c r="D34" s="3">
         <v>4</v>
       </c>
@@ -1531,14 +1620,14 @@
         <v>24</v>
       </c>
       <c r="G34" s="4"/>
-      <c r="H34" s="6"/>
-      <c r="I34" s="8"/>
-      <c r="J34" s="8"/>
+      <c r="H34" s="13"/>
+      <c r="I34" s="6"/>
+      <c r="J34" s="6"/>
     </row>
     <row r="35" spans="1:10" ht="32.25" thickBot="1">
-      <c r="A35" s="8"/>
-      <c r="B35" s="10"/>
-      <c r="C35" s="12"/>
+      <c r="A35" s="6"/>
+      <c r="B35" s="8"/>
+      <c r="C35" s="10"/>
       <c r="D35" s="3">
         <v>5</v>
       </c>
@@ -1549,14 +1638,14 @@
         <v>34</v>
       </c>
       <c r="G35" s="4"/>
-      <c r="H35" s="6"/>
-      <c r="I35" s="8"/>
-      <c r="J35" s="8"/>
+      <c r="H35" s="13"/>
+      <c r="I35" s="6"/>
+      <c r="J35" s="6"/>
     </row>
     <row r="36" spans="1:10" ht="32.25" thickBot="1">
-      <c r="A36" s="8"/>
-      <c r="B36" s="10"/>
-      <c r="C36" s="12"/>
+      <c r="A36" s="6"/>
+      <c r="B36" s="8"/>
+      <c r="C36" s="10"/>
       <c r="D36" s="3">
         <v>6</v>
       </c>
@@ -1567,14 +1656,14 @@
         <v>35</v>
       </c>
       <c r="G36" s="4"/>
-      <c r="H36" s="6"/>
-      <c r="I36" s="8"/>
-      <c r="J36" s="8"/>
+      <c r="H36" s="13"/>
+      <c r="I36" s="6"/>
+      <c r="J36" s="6"/>
     </row>
     <row r="37" spans="1:10" ht="42.75" thickBot="1">
-      <c r="A37" s="8"/>
-      <c r="B37" s="10"/>
-      <c r="C37" s="12"/>
+      <c r="A37" s="6"/>
+      <c r="B37" s="8"/>
+      <c r="C37" s="10"/>
       <c r="D37" s="3">
         <v>7</v>
       </c>
@@ -1585,9 +1674,9 @@
         <v>43</v>
       </c>
       <c r="G37" s="4"/>
-      <c r="H37" s="6"/>
-      <c r="I37" s="8"/>
-      <c r="J37" s="8"/>
+      <c r="H37" s="13"/>
+      <c r="I37" s="6"/>
+      <c r="J37" s="6"/>
     </row>
     <row r="38" spans="1:10" ht="15.75" thickBot="1">
       <c r="A38" s="1"/>
@@ -1603,11 +1692,15 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="A31:A37"/>
-    <mergeCell ref="B31:B37"/>
-    <mergeCell ref="C31:C37"/>
-    <mergeCell ref="B9:B14"/>
-    <mergeCell ref="C9:C14"/>
+    <mergeCell ref="J31:J37"/>
+    <mergeCell ref="H9:H14"/>
+    <mergeCell ref="I9:I14"/>
+    <mergeCell ref="J9:J14"/>
+    <mergeCell ref="H2:H7"/>
+    <mergeCell ref="I2:I7"/>
+    <mergeCell ref="B2:B7"/>
+    <mergeCell ref="H31:H37"/>
+    <mergeCell ref="I31:I37"/>
     <mergeCell ref="A2:A7"/>
     <mergeCell ref="C2:C7"/>
     <mergeCell ref="I16:I22"/>
@@ -1624,15 +1717,11 @@
     <mergeCell ref="C16:C22"/>
     <mergeCell ref="H16:H22"/>
     <mergeCell ref="J2:J7"/>
-    <mergeCell ref="H2:H7"/>
-    <mergeCell ref="I2:I7"/>
-    <mergeCell ref="B2:B7"/>
-    <mergeCell ref="H31:H37"/>
-    <mergeCell ref="I31:I37"/>
-    <mergeCell ref="J31:J37"/>
-    <mergeCell ref="H9:H14"/>
-    <mergeCell ref="I9:I14"/>
-    <mergeCell ref="J9:J14"/>
+    <mergeCell ref="A31:A37"/>
+    <mergeCell ref="B31:B37"/>
+    <mergeCell ref="C31:C37"/>
+    <mergeCell ref="B9:B14"/>
+    <mergeCell ref="C9:C14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1706,13 +1795,13 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="21.75" thickBot="1">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="9" t="s">
         <v>45</v>
       </c>
       <c r="D2" s="3">
@@ -1725,16 +1814,16 @@
         <v>67</v>
       </c>
       <c r="G2" s="4"/>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
     </row>
     <row r="3" spans="1:10" ht="42.75" customHeight="1" thickBot="1">
-      <c r="A3" s="8"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="12"/>
+      <c r="A3" s="6"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="10"/>
       <c r="D3" s="3">
         <v>2</v>
       </c>
@@ -1745,14 +1834,14 @@
         <v>23</v>
       </c>
       <c r="G3" s="4"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
     </row>
     <row r="4" spans="1:10" ht="21.75" thickBot="1">
-      <c r="A4" s="8"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="12"/>
+      <c r="A4" s="6"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="10"/>
       <c r="D4" s="3">
         <v>3</v>
       </c>
@@ -1763,14 +1852,14 @@
         <v>19</v>
       </c>
       <c r="G4" s="4"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
     </row>
     <row r="5" spans="1:10" ht="42.75" thickBot="1">
-      <c r="A5" s="8"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="12"/>
+      <c r="A5" s="6"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="10"/>
       <c r="D5" s="3">
         <v>4</v>
       </c>
@@ -1781,14 +1870,14 @@
         <v>24</v>
       </c>
       <c r="G5" s="4"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
     </row>
     <row r="6" spans="1:10" ht="21.75" thickBot="1">
-      <c r="A6" s="8"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="12"/>
+      <c r="A6" s="6"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="10"/>
       <c r="D6" s="3">
         <v>5</v>
       </c>
@@ -1799,14 +1888,14 @@
         <v>48</v>
       </c>
       <c r="G6" s="4"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
     </row>
     <row r="7" spans="1:10" ht="32.25" thickBot="1">
-      <c r="A7" s="8"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="12"/>
+      <c r="A7" s="6"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="10"/>
       <c r="D7" s="3">
         <v>6</v>
       </c>
@@ -1817,9 +1906,9 @@
         <v>50</v>
       </c>
       <c r="G7" s="4"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
     </row>
     <row r="8" spans="1:10" ht="15.75" thickBot="1">
       <c r="A8" s="1"/>
@@ -1834,13 +1923,13 @@
       <c r="J8" s="1"/>
     </row>
     <row r="9" spans="1:10" ht="21.75" thickBot="1">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="9" t="s">
         <v>52</v>
       </c>
       <c r="D9" s="3">
@@ -1853,16 +1942,16 @@
         <v>67</v>
       </c>
       <c r="G9" s="4"/>
-      <c r="H9" s="5" t="s">
+      <c r="H9" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="21.75" thickBot="1">
-      <c r="A10" s="8"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="12"/>
+      <c r="A10" s="6"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="10"/>
       <c r="D10" s="3">
         <v>2</v>
       </c>
@@ -1873,14 +1962,14 @@
         <v>23</v>
       </c>
       <c r="G10" s="4"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
     </row>
     <row r="11" spans="1:10" ht="21.75" thickBot="1">
-      <c r="A11" s="8"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="12"/>
+      <c r="A11" s="6"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="10"/>
       <c r="D11" s="3">
         <v>3</v>
       </c>
@@ -1891,14 +1980,14 @@
         <v>19</v>
       </c>
       <c r="G11" s="4"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
     </row>
     <row r="12" spans="1:10" ht="42.75" thickBot="1">
-      <c r="A12" s="8"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="12"/>
+      <c r="A12" s="6"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="10"/>
       <c r="D12" s="3">
         <v>4</v>
       </c>
@@ -1909,14 +1998,14 @@
         <v>24</v>
       </c>
       <c r="G12" s="4"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
     </row>
     <row r="13" spans="1:10" ht="21.75" thickBot="1">
-      <c r="A13" s="8"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="12"/>
+      <c r="A13" s="6"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="10"/>
       <c r="D13" s="3">
         <v>5</v>
       </c>
@@ -1927,14 +2016,14 @@
         <v>48</v>
       </c>
       <c r="G13" s="4"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
     </row>
     <row r="14" spans="1:10" ht="42.75" thickBot="1">
-      <c r="A14" s="8"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="12"/>
+      <c r="A14" s="6"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="10"/>
       <c r="D14" s="3">
         <v>6</v>
       </c>
@@ -1945,9 +2034,9 @@
         <v>54</v>
       </c>
       <c r="G14" s="4"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
     </row>
     <row r="15" spans="1:10" ht="15.75" thickBot="1">
       <c r="A15" s="1"/>
@@ -2001,10 +2090,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2048,13 +2137,13 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="21.75" thickBot="1">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="9" t="s">
         <v>60</v>
       </c>
       <c r="D2" s="3">
@@ -2067,16 +2156,16 @@
         <v>67</v>
       </c>
       <c r="G2" s="4"/>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
     </row>
     <row r="3" spans="1:10" ht="32.25" thickBot="1">
-      <c r="A3" s="8"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="12"/>
+      <c r="A3" s="6"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="10"/>
       <c r="D3" s="3">
         <v>2</v>
       </c>
@@ -2087,14 +2176,14 @@
         <v>57</v>
       </c>
       <c r="G3" s="4"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
     </row>
     <row r="4" spans="1:10" ht="21.75" thickBot="1">
-      <c r="A4" s="8"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="12"/>
+      <c r="A4" s="6"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="10"/>
       <c r="D4" s="3">
         <v>3</v>
       </c>
@@ -2105,14 +2194,14 @@
         <v>19</v>
       </c>
       <c r="G4" s="4"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
     </row>
     <row r="5" spans="1:10" ht="53.25" thickBot="1">
-      <c r="A5" s="8"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="12"/>
+      <c r="A5" s="6"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="10"/>
       <c r="D5" s="3">
         <v>4</v>
       </c>
@@ -2123,14 +2212,14 @@
         <v>73</v>
       </c>
       <c r="G5" s="4"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
     </row>
     <row r="6" spans="1:10" ht="21.75" thickBot="1">
-      <c r="A6" s="8"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="12"/>
+      <c r="A6" s="6"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="10"/>
       <c r="D6" s="3">
         <v>5</v>
       </c>
@@ -2141,9 +2230,9 @@
         <v>72</v>
       </c>
       <c r="G6" s="4"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
     </row>
     <row r="7" spans="1:10" ht="15.75" thickBot="1">
       <c r="A7" s="1"/>
@@ -2158,13 +2247,13 @@
       <c r="J7" s="1"/>
     </row>
     <row r="8" spans="1:10" ht="21.75" thickBot="1">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="9" t="s">
         <v>74</v>
       </c>
       <c r="D8" s="3">
@@ -2177,16 +2266,16 @@
         <v>67</v>
       </c>
       <c r="G8" s="4"/>
-      <c r="H8" s="5" t="s">
+      <c r="H8" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="32.25" thickBot="1">
-      <c r="A9" s="8"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="12"/>
+      <c r="A9" s="6"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="10"/>
       <c r="D9" s="3">
         <v>2</v>
       </c>
@@ -2197,14 +2286,14 @@
         <v>23</v>
       </c>
       <c r="G9" s="4"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
     </row>
     <row r="10" spans="1:10" ht="21.75" thickBot="1">
-      <c r="A10" s="8"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="12"/>
+      <c r="A10" s="6"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="10"/>
       <c r="D10" s="3">
         <v>3</v>
       </c>
@@ -2215,14 +2304,14 @@
         <v>19</v>
       </c>
       <c r="G10" s="4"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
     </row>
     <row r="11" spans="1:10" ht="42.75" thickBot="1">
-      <c r="A11" s="8"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="12"/>
+      <c r="A11" s="6"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="10"/>
       <c r="D11" s="3">
         <v>4</v>
       </c>
@@ -2233,9 +2322,9 @@
         <v>76</v>
       </c>
       <c r="G11" s="4"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
     </row>
     <row r="12" spans="1:10" ht="15.75" thickBot="1">
       <c r="A12" s="1"/>
@@ -2250,13 +2339,13 @@
       <c r="J12" s="1"/>
     </row>
     <row r="13" spans="1:10" ht="21.75" thickBot="1">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="9" t="s">
         <v>79</v>
       </c>
       <c r="D13" s="3">
@@ -2269,16 +2358,16 @@
         <v>67</v>
       </c>
       <c r="G13" s="4"/>
-      <c r="H13" s="5" t="s">
+      <c r="H13" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10" ht="32.25" thickBot="1">
-      <c r="A14" s="8"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="12"/>
+      <c r="A14" s="6"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="10"/>
       <c r="D14" s="3">
         <v>2</v>
       </c>
@@ -2289,14 +2378,14 @@
         <v>57</v>
       </c>
       <c r="G14" s="4"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
     </row>
     <row r="15" spans="1:10" ht="21.75" thickBot="1">
-      <c r="A15" s="8"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="12"/>
+      <c r="A15" s="6"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="10"/>
       <c r="D15" s="3">
         <v>3</v>
       </c>
@@ -2307,14 +2396,14 @@
         <v>19</v>
       </c>
       <c r="G15" s="4"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10" ht="63.75" thickBot="1">
-      <c r="A16" s="8"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="12"/>
+      <c r="A16" s="6"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="10"/>
       <c r="D16" s="3">
         <v>4</v>
       </c>
@@ -2325,9 +2414,9 @@
         <v>80</v>
       </c>
       <c r="G16" s="4"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
     </row>
     <row r="17" spans="1:10" ht="15.75" thickBot="1">
       <c r="A17" s="1"/>
@@ -2342,13 +2431,13 @@
       <c r="J17" s="1"/>
     </row>
     <row r="18" spans="1:10" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C18" s="9" t="s">
         <v>91</v>
       </c>
       <c r="D18" s="3">
@@ -2361,16 +2450,16 @@
         <v>67</v>
       </c>
       <c r="G18" s="4"/>
-      <c r="H18" s="5" t="s">
+      <c r="H18" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
     </row>
     <row r="19" spans="1:10" ht="32.25" thickBot="1">
-      <c r="A19" s="8"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="12"/>
+      <c r="A19" s="6"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="10"/>
       <c r="D19" s="3">
         <v>2</v>
       </c>
@@ -2381,14 +2470,14 @@
         <v>57</v>
       </c>
       <c r="G19" s="4"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
     </row>
     <row r="20" spans="1:10" ht="21.75" thickBot="1">
-      <c r="A20" s="8"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="12"/>
+      <c r="A20" s="6"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="10"/>
       <c r="D20" s="3">
         <v>3</v>
       </c>
@@ -2399,14 +2488,14 @@
         <v>19</v>
       </c>
       <c r="G20" s="4"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="8"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
     </row>
     <row r="21" spans="1:10" ht="21.75" thickBot="1">
-      <c r="A21" s="8"/>
-      <c r="B21" s="10"/>
-      <c r="C21" s="12"/>
+      <c r="A21" s="6"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="10"/>
       <c r="D21" s="3">
         <v>4</v>
       </c>
@@ -2417,14 +2506,14 @@
         <v>83</v>
       </c>
       <c r="G21" s="4"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="8"/>
-      <c r="J21" s="8"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
     </row>
     <row r="22" spans="1:10" ht="95.25" thickBot="1">
-      <c r="A22" s="8"/>
-      <c r="B22" s="10"/>
-      <c r="C22" s="12"/>
+      <c r="A22" s="6"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="10"/>
       <c r="D22" s="3">
         <v>5</v>
       </c>
@@ -2435,14 +2524,14 @@
         <v>85</v>
       </c>
       <c r="G22" s="4"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="8"/>
-      <c r="J22" s="8"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
     </row>
     <row r="23" spans="1:10" ht="21.75" thickBot="1">
-      <c r="A23" s="8"/>
-      <c r="B23" s="10"/>
-      <c r="C23" s="12"/>
+      <c r="A23" s="6"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="10"/>
       <c r="D23" s="3">
         <v>6</v>
       </c>
@@ -2453,14 +2542,14 @@
         <v>87</v>
       </c>
       <c r="G23" s="4"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="8"/>
-      <c r="J23" s="8"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
     </row>
     <row r="24" spans="1:10" ht="32.25" thickBot="1">
-      <c r="A24" s="8"/>
-      <c r="B24" s="10"/>
-      <c r="C24" s="12"/>
+      <c r="A24" s="6"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="10"/>
       <c r="D24" s="3">
         <v>7</v>
       </c>
@@ -2469,14 +2558,14 @@
       </c>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="8"/>
-      <c r="J24" s="8"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
     </row>
     <row r="25" spans="1:10" ht="21.75" thickBot="1">
-      <c r="A25" s="8"/>
-      <c r="B25" s="10"/>
-      <c r="C25" s="12"/>
+      <c r="A25" s="6"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="10"/>
       <c r="D25" s="3">
         <v>8</v>
       </c>
@@ -2485,14 +2574,14 @@
       </c>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="8"/>
-      <c r="J25" s="8"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="6"/>
     </row>
     <row r="26" spans="1:10" ht="42.75" thickBot="1">
-      <c r="A26" s="8"/>
-      <c r="B26" s="10"/>
-      <c r="C26" s="12"/>
+      <c r="A26" s="6"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="10"/>
       <c r="D26" s="3">
         <v>9</v>
       </c>
@@ -2501,14 +2590,14 @@
       </c>
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="8"/>
-      <c r="J26" s="8"/>
+      <c r="H26" s="13"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="21.75" thickBot="1">
-      <c r="A27" s="8"/>
-      <c r="B27" s="10"/>
-      <c r="C27" s="12"/>
+      <c r="A27" s="6"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="10"/>
       <c r="D27" s="3">
         <v>10</v>
       </c>
@@ -2519,9 +2608,9 @@
         <v>93</v>
       </c>
       <c r="G27" s="4"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="8"/>
-      <c r="J27" s="8"/>
+      <c r="H27" s="13"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="15.75" thickBot="1">
       <c r="A28" s="1"/>
@@ -2535,20 +2624,210 @@
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
     </row>
+    <row r="29" spans="1:10" ht="21.75" thickBot="1">
+      <c r="A29" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="D29" s="3">
+        <v>1</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G29" s="4"/>
+      <c r="H29" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="I29" s="5"/>
+      <c r="J29" s="5"/>
+    </row>
+    <row r="30" spans="1:10" ht="32.25" thickBot="1">
+      <c r="A30" s="6"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="3">
+        <v>2</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="G30" s="4"/>
+      <c r="H30" s="13"/>
+      <c r="I30" s="6"/>
+      <c r="J30" s="6"/>
+    </row>
+    <row r="31" spans="1:10" ht="21.75" thickBot="1">
+      <c r="A31" s="6"/>
+      <c r="B31" s="8"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="3">
+        <v>3</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G31" s="4"/>
+      <c r="H31" s="13"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="6"/>
+    </row>
+    <row r="32" spans="1:10" ht="21.75" thickBot="1">
+      <c r="A32" s="6"/>
+      <c r="B32" s="8"/>
+      <c r="C32" s="10"/>
+      <c r="D32" s="3">
+        <v>4</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="G32" s="4"/>
+      <c r="H32" s="13"/>
+      <c r="I32" s="6"/>
+      <c r="J32" s="6"/>
+    </row>
+    <row r="33" spans="1:10" ht="95.25" thickBot="1">
+      <c r="A33" s="6"/>
+      <c r="B33" s="8"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="3">
+        <v>5</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G33" s="4"/>
+      <c r="H33" s="13"/>
+      <c r="I33" s="6"/>
+      <c r="J33" s="6"/>
+    </row>
+    <row r="34" spans="1:10" ht="21.75" thickBot="1">
+      <c r="A34" s="6"/>
+      <c r="B34" s="8"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="3">
+        <v>6</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="G34" s="4"/>
+      <c r="H34" s="13"/>
+      <c r="I34" s="6"/>
+      <c r="J34" s="6"/>
+    </row>
+    <row r="35" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A35" s="6"/>
+      <c r="B35" s="8"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="3">
+        <v>7</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="G35" s="4"/>
+      <c r="H35" s="13"/>
+      <c r="I35" s="6"/>
+      <c r="J35" s="6"/>
+    </row>
+    <row r="36" spans="1:10" ht="21.75" thickBot="1">
+      <c r="A36" s="6"/>
+      <c r="B36" s="8"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="3">
+        <v>8</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
+      <c r="H36" s="13"/>
+      <c r="I36" s="6"/>
+      <c r="J36" s="6"/>
+    </row>
+    <row r="37" spans="1:10" ht="42.75" thickBot="1">
+      <c r="A37" s="6"/>
+      <c r="B37" s="8"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="3">
+        <v>9</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
+      <c r="H37" s="13"/>
+      <c r="I37" s="6"/>
+      <c r="J37" s="6"/>
+    </row>
+    <row r="38" spans="1:10" ht="21.75" thickBot="1">
+      <c r="A38" s="6"/>
+      <c r="B38" s="8"/>
+      <c r="C38" s="10"/>
+      <c r="D38" s="3">
+        <v>10</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="G38" s="4"/>
+      <c r="H38" s="13"/>
+      <c r="I38" s="6"/>
+      <c r="J38" s="6"/>
+    </row>
+    <row r="39" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+      <c r="J39" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="24">
-    <mergeCell ref="A18:A27"/>
-    <mergeCell ref="J18:J27"/>
-    <mergeCell ref="I18:I27"/>
-    <mergeCell ref="H18:H27"/>
-    <mergeCell ref="C18:C27"/>
-    <mergeCell ref="B18:B27"/>
-    <mergeCell ref="J13:J16"/>
-    <mergeCell ref="A13:A16"/>
-    <mergeCell ref="B13:B16"/>
-    <mergeCell ref="C13:C16"/>
-    <mergeCell ref="H13:H16"/>
-    <mergeCell ref="I13:I16"/>
+  <mergeCells count="30">
+    <mergeCell ref="J29:J38"/>
+    <mergeCell ref="A29:A38"/>
+    <mergeCell ref="B29:B38"/>
+    <mergeCell ref="C29:C38"/>
+    <mergeCell ref="H29:H38"/>
+    <mergeCell ref="I29:I38"/>
     <mergeCell ref="J2:J6"/>
     <mergeCell ref="A8:A11"/>
     <mergeCell ref="B8:B11"/>
@@ -2561,6 +2840,18 @@
     <mergeCell ref="C2:C6"/>
     <mergeCell ref="H2:H6"/>
     <mergeCell ref="I2:I6"/>
+    <mergeCell ref="J13:J16"/>
+    <mergeCell ref="A13:A16"/>
+    <mergeCell ref="B13:B16"/>
+    <mergeCell ref="C13:C16"/>
+    <mergeCell ref="H13:H16"/>
+    <mergeCell ref="I13:I16"/>
+    <mergeCell ref="A18:A27"/>
+    <mergeCell ref="J18:J27"/>
+    <mergeCell ref="I18:I27"/>
+    <mergeCell ref="H18:H27"/>
+    <mergeCell ref="C18:C27"/>
+    <mergeCell ref="B18:B27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2571,13 +2862,13 @@
           <x14:formula1>
             <xm:f>Reference!$A$1:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>H2:H6 H8:H11 H13:H16 H18:H27</xm:sqref>
+          <xm:sqref>H2:H6 H8:H11 H13:H16 H18:H27 H29:H38</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Reference!$C$1:$C$4</xm:f>
           </x14:formula1>
-          <xm:sqref>I2:I6 I8:I11 I13:I16 I18:I27</xm:sqref>
+          <xm:sqref>I2:I6 I8:I11 I13:I16 I18:I27 I29:I38</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2587,10 +2878,832 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J42"/>
+  <sheetViews>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="5" max="5" width="23.42578125" customWidth="1"/>
+    <col min="6" max="6" width="27.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="21.75" thickBot="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="21.75" thickBot="1">
+      <c r="A2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="D2" s="3">
+        <v>1</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G2" s="4"/>
+      <c r="H2" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+    </row>
+    <row r="3" spans="1:10" ht="32.25" thickBot="1">
+      <c r="A3" s="6"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="3">
+        <v>2</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="4"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+    </row>
+    <row r="4" spans="1:10" ht="21.75" thickBot="1">
+      <c r="A4" s="6"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="3">
+        <v>3</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="4"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+    </row>
+    <row r="5" spans="1:10" ht="42.75" thickBot="1">
+      <c r="A5" s="6"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="3">
+        <v>4</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="4"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+    </row>
+    <row r="6" spans="1:10" ht="84.75" thickBot="1">
+      <c r="A6" s="6"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="3">
+        <v>5</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="G6" s="4"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+    </row>
+    <row r="7" spans="1:10" ht="32.25" thickBot="1">
+      <c r="A7" s="6"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="3">
+        <v>6</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+    </row>
+    <row r="8" spans="1:10" ht="21.75" thickBot="1">
+      <c r="A8" s="6"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="3">
+        <v>7</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+    </row>
+    <row r="9" spans="1:10" ht="32.25" thickBot="1">
+      <c r="A9" s="6"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="3">
+        <v>8</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+    </row>
+    <row r="10" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+    </row>
+    <row r="11" spans="1:10" ht="21.75" thickBot="1">
+      <c r="A11" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="D11" s="3">
+        <v>1</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G11" s="4"/>
+      <c r="H11" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+    </row>
+    <row r="12" spans="1:10" ht="32.25" thickBot="1">
+      <c r="A12" s="6"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="3">
+        <v>2</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" s="4"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+    </row>
+    <row r="13" spans="1:10" ht="21.75" thickBot="1">
+      <c r="A13" s="6"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="3">
+        <v>3</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G13" s="4"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+    </row>
+    <row r="14" spans="1:10" ht="42.75" thickBot="1">
+      <c r="A14" s="6"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="3">
+        <v>4</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G14" s="4"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+    </row>
+    <row r="15" spans="1:10" ht="84.75" thickBot="1">
+      <c r="A15" s="6"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="3">
+        <v>5</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="G15" s="4"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+    </row>
+    <row r="16" spans="1:10" ht="32.25" thickBot="1">
+      <c r="A16" s="6"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="3">
+        <v>6</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+    </row>
+    <row r="17" spans="1:10" ht="21.75" thickBot="1">
+      <c r="A17" s="6"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="3">
+        <v>7</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+    </row>
+    <row r="18" spans="1:10" ht="32.25" thickBot="1">
+      <c r="A18" s="6"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="3">
+        <v>8</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+    </row>
+    <row r="19" spans="1:10" ht="32.25" thickBot="1">
+      <c r="A19" s="6"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="3">
+        <v>9</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="G19" s="4"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+    </row>
+    <row r="20" spans="1:10" ht="42.75" thickBot="1">
+      <c r="A20" s="6"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="3">
+        <v>10</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="G20" s="4"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+    </row>
+    <row r="21" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+    </row>
+    <row r="22" spans="1:10" ht="21.75" customHeight="1" thickBot="1">
+      <c r="A22" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="D22" s="3">
+        <v>1</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G22" s="4"/>
+      <c r="H22" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+    </row>
+    <row r="23" spans="1:10" ht="32.25" thickBot="1">
+      <c r="A23" s="6"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="3">
+        <v>2</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G23" s="4"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+    </row>
+    <row r="24" spans="1:10" ht="21.75" thickBot="1">
+      <c r="A24" s="6"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="3">
+        <v>3</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G24" s="4"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+    </row>
+    <row r="25" spans="1:10" ht="42.75" thickBot="1">
+      <c r="A25" s="6"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="3">
+        <v>4</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G25" s="4"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="6"/>
+    </row>
+    <row r="26" spans="1:10" ht="84.75" thickBot="1">
+      <c r="A26" s="6"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="3">
+        <v>5</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="G26" s="4"/>
+      <c r="H26" s="13"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6"/>
+    </row>
+    <row r="27" spans="1:10" ht="21.75" thickBot="1">
+      <c r="A27" s="6"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="3">
+        <v>6</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="G27" s="4"/>
+      <c r="H27" s="13"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="6"/>
+    </row>
+    <row r="28" spans="1:10" ht="32.25" thickBot="1">
+      <c r="A28" s="6"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="3">
+        <v>7</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="13"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="6"/>
+    </row>
+    <row r="29" spans="1:10" ht="21.75" thickBot="1">
+      <c r="A29" s="6"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="3">
+        <v>8</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="G29" s="4"/>
+      <c r="H29" s="13"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="6"/>
+    </row>
+    <row r="30" spans="1:10" ht="32.25" thickBot="1">
+      <c r="A30" s="6"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="3">
+        <v>9</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="13"/>
+      <c r="I30" s="6"/>
+      <c r="J30" s="6"/>
+    </row>
+    <row r="31" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+    </row>
+    <row r="32" spans="1:10" ht="21.75" thickBot="1">
+      <c r="A32" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="D32" s="3">
+        <v>1</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G32" s="4"/>
+      <c r="H32" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="I32" s="5"/>
+      <c r="J32" s="5"/>
+    </row>
+    <row r="33" spans="1:10" ht="32.25" thickBot="1">
+      <c r="A33" s="6"/>
+      <c r="B33" s="8"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="3">
+        <v>2</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G33" s="4"/>
+      <c r="H33" s="13"/>
+      <c r="I33" s="6"/>
+      <c r="J33" s="6"/>
+    </row>
+    <row r="34" spans="1:10" ht="21.75" thickBot="1">
+      <c r="A34" s="6"/>
+      <c r="B34" s="8"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="3">
+        <v>3</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G34" s="4"/>
+      <c r="H34" s="13"/>
+      <c r="I34" s="6"/>
+      <c r="J34" s="6"/>
+    </row>
+    <row r="35" spans="1:10" ht="42.75" thickBot="1">
+      <c r="A35" s="6"/>
+      <c r="B35" s="8"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="3">
+        <v>4</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G35" s="4"/>
+      <c r="H35" s="13"/>
+      <c r="I35" s="6"/>
+      <c r="J35" s="6"/>
+    </row>
+    <row r="36" spans="1:10" ht="84.75" thickBot="1">
+      <c r="A36" s="6"/>
+      <c r="B36" s="8"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="3">
+        <v>5</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="G36" s="4"/>
+      <c r="H36" s="13"/>
+      <c r="I36" s="6"/>
+      <c r="J36" s="6"/>
+    </row>
+    <row r="37" spans="1:10" ht="21.75" thickBot="1">
+      <c r="A37" s="6"/>
+      <c r="B37" s="8"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="3">
+        <v>6</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="G37" s="4"/>
+      <c r="H37" s="13"/>
+      <c r="I37" s="6"/>
+      <c r="J37" s="6"/>
+    </row>
+    <row r="38" spans="1:10" ht="32.25" thickBot="1">
+      <c r="A38" s="6"/>
+      <c r="B38" s="8"/>
+      <c r="C38" s="10"/>
+      <c r="D38" s="3">
+        <v>7</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4"/>
+      <c r="H38" s="13"/>
+      <c r="I38" s="6"/>
+      <c r="J38" s="6"/>
+    </row>
+    <row r="39" spans="1:10" ht="21.75" thickBot="1">
+      <c r="A39" s="6"/>
+      <c r="B39" s="8"/>
+      <c r="C39" s="10"/>
+      <c r="D39" s="3">
+        <v>8</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="G39" s="4"/>
+      <c r="H39" s="13"/>
+      <c r="I39" s="6"/>
+      <c r="J39" s="6"/>
+    </row>
+    <row r="40" spans="1:10" ht="32.25" thickBot="1">
+      <c r="A40" s="6"/>
+      <c r="B40" s="8"/>
+      <c r="C40" s="10"/>
+      <c r="D40" s="3">
+        <v>9</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="F40" s="4"/>
+      <c r="G40" s="4"/>
+      <c r="H40" s="13"/>
+      <c r="I40" s="6"/>
+      <c r="J40" s="6"/>
+    </row>
+    <row r="41" spans="1:10" ht="42.75" thickBot="1">
+      <c r="A41" s="6"/>
+      <c r="B41" s="8"/>
+      <c r="C41" s="10"/>
+      <c r="D41" s="3">
+        <v>10</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="G41" s="4"/>
+      <c r="H41" s="13"/>
+      <c r="I41" s="6"/>
+      <c r="J41" s="6"/>
+    </row>
+    <row r="42" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A42" s="1"/>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
+      <c r="H42" s="1"/>
+      <c r="I42" s="1"/>
+      <c r="J42" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="24">
+    <mergeCell ref="J22:J30"/>
+    <mergeCell ref="A32:A41"/>
+    <mergeCell ref="B32:B41"/>
+    <mergeCell ref="C32:C41"/>
+    <mergeCell ref="H32:H41"/>
+    <mergeCell ref="I32:I41"/>
+    <mergeCell ref="J32:J41"/>
+    <mergeCell ref="A22:A30"/>
+    <mergeCell ref="B22:B30"/>
+    <mergeCell ref="C22:C30"/>
+    <mergeCell ref="H22:H30"/>
+    <mergeCell ref="I22:I30"/>
+    <mergeCell ref="I2:I9"/>
+    <mergeCell ref="J2:J9"/>
+    <mergeCell ref="A11:A20"/>
+    <mergeCell ref="B11:B20"/>
+    <mergeCell ref="C11:C20"/>
+    <mergeCell ref="H11:H20"/>
+    <mergeCell ref="I11:I20"/>
+    <mergeCell ref="J11:J20"/>
+    <mergeCell ref="A2:A9"/>
+    <mergeCell ref="B2:B9"/>
+    <mergeCell ref="C2:C9"/>
+    <mergeCell ref="H2:H9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Reference!$A$1:$A$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>H2:H9 H11:H20 H22:H30 H32:H41</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Reference!$C$1:$C$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>I2:I9 I11:I20 I22:I30 I32:I41</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:J13"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2628,13 +3741,13 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="63.75" thickBot="1">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="C2" s="11" t="s">
+      <c r="B2" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="C2" s="9" t="s">
         <v>45</v>
       </c>
       <c r="D2" s="3">
@@ -2647,16 +3760,16 @@
         <v>23</v>
       </c>
       <c r="G2" s="4"/>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
     </row>
     <row r="3" spans="1:10" ht="42.75" thickBot="1">
-      <c r="A3" s="8"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="12"/>
+      <c r="A3" s="6"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="10"/>
       <c r="D3" s="3">
         <v>2</v>
       </c>
@@ -2667,14 +3780,14 @@
         <v>19</v>
       </c>
       <c r="G3" s="4"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
     </row>
     <row r="4" spans="1:10" ht="105.75" thickBot="1">
-      <c r="A4" s="8"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="12"/>
+      <c r="A4" s="6"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="10"/>
       <c r="D4" s="3">
         <v>3</v>
       </c>
@@ -2685,14 +3798,14 @@
         <v>24</v>
       </c>
       <c r="G4" s="4"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
     </row>
     <row r="5" spans="1:10" ht="74.25" thickBot="1">
-      <c r="A5" s="8"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="12"/>
+      <c r="A5" s="6"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="10"/>
       <c r="D5" s="3">
         <v>4</v>
       </c>
@@ -2703,14 +3816,14 @@
         <v>48</v>
       </c>
       <c r="G5" s="4"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
     </row>
     <row r="6" spans="1:10" ht="74.25" thickBot="1">
-      <c r="A6" s="8"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="12"/>
+      <c r="A6" s="6"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="10"/>
       <c r="D6" s="3">
         <v>5</v>
       </c>
@@ -2721,9 +3834,9 @@
         <v>50</v>
       </c>
       <c r="G6" s="4"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
     </row>
     <row r="7" spans="1:10" ht="15.75" thickBot="1">
       <c r="A7" s="1"/>
@@ -2738,13 +3851,13 @@
       <c r="J7" s="1"/>
     </row>
     <row r="8" spans="1:10" ht="63.75" thickBot="1">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="C8" s="11" t="s">
+      <c r="B8" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="C8" s="9" t="s">
         <v>52</v>
       </c>
       <c r="D8" s="3">
@@ -2757,16 +3870,16 @@
         <v>23</v>
       </c>
       <c r="G8" s="4"/>
-      <c r="H8" s="5" t="s">
+      <c r="H8" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="42.75" thickBot="1">
-      <c r="A9" s="8"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="12"/>
+      <c r="A9" s="6"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="10"/>
       <c r="D9" s="3">
         <v>2</v>
       </c>
@@ -2777,14 +3890,14 @@
         <v>19</v>
       </c>
       <c r="G9" s="4"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
     </row>
     <row r="10" spans="1:10" ht="105.75" thickBot="1">
-      <c r="A10" s="8"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="12"/>
+      <c r="A10" s="6"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="10"/>
       <c r="D10" s="3">
         <v>3</v>
       </c>
@@ -2795,14 +3908,14 @@
         <v>24</v>
       </c>
       <c r="G10" s="4"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
     </row>
     <row r="11" spans="1:10" ht="74.25" thickBot="1">
-      <c r="A11" s="8"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="12"/>
+      <c r="A11" s="6"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="10"/>
       <c r="D11" s="3">
         <v>4</v>
       </c>
@@ -2813,14 +3926,14 @@
         <v>48</v>
       </c>
       <c r="G11" s="4"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
     </row>
     <row r="12" spans="1:10" ht="95.25" thickBot="1">
-      <c r="A12" s="8"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="12"/>
+      <c r="A12" s="6"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="10"/>
       <c r="D12" s="3">
         <v>5</v>
       </c>
@@ -2831,308 +3944,9 @@
         <v>54</v>
       </c>
       <c r="G12" s="4"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
-    </row>
-    <row r="13" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-    </row>
-  </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="I2:I6"/>
-    <mergeCell ref="J2:J6"/>
-    <mergeCell ref="A8:A12"/>
-    <mergeCell ref="B8:B12"/>
-    <mergeCell ref="C8:C12"/>
-    <mergeCell ref="H8:H12"/>
-    <mergeCell ref="I8:I12"/>
-    <mergeCell ref="J8:J12"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="B2:B6"/>
-    <mergeCell ref="C2:C6"/>
-    <mergeCell ref="H2:H6"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Reference!$A$1:$A$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>H2:H6 H8:H12</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Reference!$C$1:$C$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>I2:I6 I8:I12</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:J13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:10" ht="21.75" thickBot="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="63.75" thickBot="1">
-      <c r="A2" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="D2" s="3">
-        <v>1</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" s="4"/>
-      <c r="H2" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-    </row>
-    <row r="3" spans="1:10" ht="42.75" thickBot="1">
-      <c r="A3" s="8"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="3">
-        <v>2</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="4"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-    </row>
-    <row r="4" spans="1:10" ht="105.75" thickBot="1">
-      <c r="A4" s="8"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="3">
-        <v>3</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4" s="4"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-    </row>
-    <row r="5" spans="1:10" ht="74.25" thickBot="1">
-      <c r="A5" s="8"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="3">
-        <v>4</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="G5" s="4"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-    </row>
-    <row r="6" spans="1:10" ht="74.25" thickBot="1">
-      <c r="A6" s="8"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="3">
-        <v>5</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="G6" s="4"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-    </row>
-    <row r="7" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-    </row>
-    <row r="8" spans="1:10" ht="63.75" thickBot="1">
-      <c r="A8" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="D8" s="3">
-        <v>1</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G8" s="4"/>
-      <c r="H8" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-    </row>
-    <row r="9" spans="1:10" ht="42.75" thickBot="1">
-      <c r="A9" s="8"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="3">
-        <v>2</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G9" s="4"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-    </row>
-    <row r="10" spans="1:10" ht="105.75" thickBot="1">
-      <c r="A10" s="8"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="3">
-        <v>3</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G10" s="4"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-    </row>
-    <row r="11" spans="1:10" ht="74.25" thickBot="1">
-      <c r="A11" s="8"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="3">
-        <v>4</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="G11" s="4"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
-    </row>
-    <row r="12" spans="1:10" ht="95.25" thickBot="1">
-      <c r="A12" s="8"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="3">
-        <v>5</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="G12" s="4"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
     </row>
     <row r="13" spans="1:10" ht="15.75" thickBot="1">
       <c r="A13" s="1"/>
@@ -3187,8 +4001,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3226,13 +4040,13 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="63.75" thickBot="1">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="9" t="s">
         <v>45</v>
       </c>
       <c r="D2" s="3">
@@ -3245,16 +4059,16 @@
         <v>23</v>
       </c>
       <c r="G2" s="4"/>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
     </row>
     <row r="3" spans="1:10" ht="42.75" thickBot="1">
-      <c r="A3" s="8"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="12"/>
+      <c r="A3" s="6"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="10"/>
       <c r="D3" s="3">
         <v>2</v>
       </c>
@@ -3265,14 +4079,14 @@
         <v>19</v>
       </c>
       <c r="G3" s="4"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
     </row>
     <row r="4" spans="1:10" ht="105.75" thickBot="1">
-      <c r="A4" s="8"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="12"/>
+      <c r="A4" s="6"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="10"/>
       <c r="D4" s="3">
         <v>3</v>
       </c>
@@ -3283,14 +4097,14 @@
         <v>24</v>
       </c>
       <c r="G4" s="4"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
     </row>
     <row r="5" spans="1:10" ht="74.25" thickBot="1">
-      <c r="A5" s="8"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="12"/>
+      <c r="A5" s="6"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="10"/>
       <c r="D5" s="3">
         <v>4</v>
       </c>
@@ -3301,14 +4115,14 @@
         <v>48</v>
       </c>
       <c r="G5" s="4"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
     </row>
     <row r="6" spans="1:10" ht="74.25" thickBot="1">
-      <c r="A6" s="8"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="12"/>
+      <c r="A6" s="6"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="10"/>
       <c r="D6" s="3">
         <v>5</v>
       </c>
@@ -3319,9 +4133,9 @@
         <v>50</v>
       </c>
       <c r="G6" s="4"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
     </row>
     <row r="7" spans="1:10" ht="15.75" thickBot="1">
       <c r="A7" s="1"/>
@@ -3336,13 +4150,13 @@
       <c r="J7" s="1"/>
     </row>
     <row r="8" spans="1:10" ht="63.75" thickBot="1">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="9" t="s">
         <v>52</v>
       </c>
       <c r="D8" s="3">
@@ -3355,16 +4169,16 @@
         <v>23</v>
       </c>
       <c r="G8" s="4"/>
-      <c r="H8" s="5" t="s">
+      <c r="H8" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="42.75" thickBot="1">
-      <c r="A9" s="8"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="12"/>
+      <c r="A9" s="6"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="10"/>
       <c r="D9" s="3">
         <v>2</v>
       </c>
@@ -3375,14 +4189,14 @@
         <v>19</v>
       </c>
       <c r="G9" s="4"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
     </row>
     <row r="10" spans="1:10" ht="105.75" thickBot="1">
-      <c r="A10" s="8"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="12"/>
+      <c r="A10" s="6"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="10"/>
       <c r="D10" s="3">
         <v>3</v>
       </c>
@@ -3393,14 +4207,14 @@
         <v>24</v>
       </c>
       <c r="G10" s="4"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
     </row>
     <row r="11" spans="1:10" ht="74.25" thickBot="1">
-      <c r="A11" s="8"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="12"/>
+      <c r="A11" s="6"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="10"/>
       <c r="D11" s="3">
         <v>4</v>
       </c>
@@ -3411,14 +4225,14 @@
         <v>48</v>
       </c>
       <c r="G11" s="4"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
     </row>
     <row r="12" spans="1:10" ht="95.25" thickBot="1">
-      <c r="A12" s="8"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="12"/>
+      <c r="A12" s="6"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="10"/>
       <c r="D12" s="3">
         <v>5</v>
       </c>
@@ -3429,9 +4243,9 @@
         <v>54</v>
       </c>
       <c r="G12" s="4"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
     </row>
     <row r="13" spans="1:10" ht="15.75" thickBot="1">
       <c r="A13" s="1"/>

</xml_diff>

<commit_message>
Pablo: test cases para US 3
</commit_message>
<xml_diff>
--- a/Docs/08-Prueba/Tests Cases - Modulo de Planificación.xlsx
+++ b/Docs/08-Prueba/Tests Cases - Modulo de Planificación.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="127">
   <si>
     <t>Application</t>
   </si>
@@ -446,7 +446,32 @@
     <t>TC1_US3</t>
   </si>
   <si>
-    <t>TC2_US3</t>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Seleccionar la opción de </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>Planificación</t>
+    </r>
+  </si>
+  <si>
+    <t>Se muestra la planificación de dicha asignatura y la fecha de inicio y fin de la misma.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seleccionar la opción "Consultar" de uno de los contenidos mostrados. </t>
+  </si>
+  <si>
+    <t>El sistema despliega el plan de la misma</t>
   </si>
 </sst>
 </file>
@@ -590,7 +615,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -610,6 +635,12 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -625,11 +656,8 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1028,10 +1056,10 @@
       <c r="A2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="11" t="s">
         <v>21</v>
       </c>
       <c r="D2" s="3">
@@ -1044,14 +1072,14 @@
         <v>67</v>
       </c>
       <c r="G2" s="4"/>
-      <c r="H2" s="12"/>
+      <c r="H2" s="7"/>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
     </row>
     <row r="3" spans="1:10" ht="21.75" thickBot="1">
       <c r="A3" s="6"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="10"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="12"/>
       <c r="D3" s="3">
         <v>2</v>
       </c>
@@ -1062,14 +1090,14 @@
         <v>23</v>
       </c>
       <c r="G3" s="4"/>
-      <c r="H3" s="13"/>
+      <c r="H3" s="8"/>
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
     </row>
     <row r="4" spans="1:10" ht="21.75" thickBot="1">
       <c r="A4" s="6"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="10"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="12"/>
       <c r="D4" s="3">
         <v>3</v>
       </c>
@@ -1080,14 +1108,14 @@
         <v>19</v>
       </c>
       <c r="G4" s="4"/>
-      <c r="H4" s="13"/>
+      <c r="H4" s="8"/>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
     </row>
     <row r="5" spans="1:10" ht="42.75" thickBot="1">
       <c r="A5" s="6"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="10"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="12"/>
       <c r="D5" s="3">
         <v>4</v>
       </c>
@@ -1098,14 +1126,14 @@
         <v>24</v>
       </c>
       <c r="G5" s="4"/>
-      <c r="H5" s="13"/>
+      <c r="H5" s="8"/>
       <c r="I5" s="6"/>
       <c r="J5" s="6"/>
     </row>
     <row r="6" spans="1:10" ht="21.75" thickBot="1">
       <c r="A6" s="6"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="10"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="12"/>
       <c r="D6" s="3">
         <v>5</v>
       </c>
@@ -1116,14 +1144,14 @@
         <v>25</v>
       </c>
       <c r="G6" s="4"/>
-      <c r="H6" s="13"/>
+      <c r="H6" s="8"/>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
     </row>
     <row r="7" spans="1:10" ht="42.75" thickBot="1">
       <c r="A7" s="6"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="10"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="12"/>
       <c r="D7" s="3">
         <v>6</v>
       </c>
@@ -1134,7 +1162,7 @@
         <v>27</v>
       </c>
       <c r="G7" s="4"/>
-      <c r="H7" s="13"/>
+      <c r="H7" s="8"/>
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
     </row>
@@ -1154,10 +1182,10 @@
       <c r="A9" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="11" t="s">
         <v>29</v>
       </c>
       <c r="D9" s="3">
@@ -1170,14 +1198,14 @@
         <v>67</v>
       </c>
       <c r="G9" s="4"/>
-      <c r="H9" s="12"/>
+      <c r="H9" s="7"/>
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="21.75" customHeight="1" thickBot="1">
       <c r="A10" s="6"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="10"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="12"/>
       <c r="D10" s="3">
         <v>2</v>
       </c>
@@ -1188,14 +1216,14 @@
         <v>23</v>
       </c>
       <c r="G10" s="4"/>
-      <c r="H10" s="13"/>
+      <c r="H10" s="8"/>
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
     </row>
     <row r="11" spans="1:10" ht="21.75" thickBot="1">
       <c r="A11" s="6"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="10"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="12"/>
       <c r="D11" s="3">
         <v>3</v>
       </c>
@@ -1206,14 +1234,14 @@
         <v>19</v>
       </c>
       <c r="G11" s="4"/>
-      <c r="H11" s="13"/>
+      <c r="H11" s="8"/>
       <c r="I11" s="6"/>
       <c r="J11" s="6"/>
     </row>
     <row r="12" spans="1:10" ht="42.75" thickBot="1">
       <c r="A12" s="6"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="10"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="12"/>
       <c r="D12" s="3">
         <v>4</v>
       </c>
@@ -1224,14 +1252,14 @@
         <v>24</v>
       </c>
       <c r="G12" s="4"/>
-      <c r="H12" s="13"/>
+      <c r="H12" s="8"/>
       <c r="I12" s="6"/>
       <c r="J12" s="6"/>
     </row>
     <row r="13" spans="1:10" ht="21.75" thickBot="1">
       <c r="A13" s="6"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="10"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="12"/>
       <c r="D13" s="3">
         <v>5</v>
       </c>
@@ -1242,14 +1270,14 @@
         <v>25</v>
       </c>
       <c r="G13" s="4"/>
-      <c r="H13" s="13"/>
+      <c r="H13" s="8"/>
       <c r="I13" s="6"/>
       <c r="J13" s="6"/>
     </row>
     <row r="14" spans="1:10" ht="42.75" thickBot="1">
       <c r="A14" s="6"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="11"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="13"/>
       <c r="D14" s="3">
         <v>6</v>
       </c>
@@ -1260,7 +1288,7 @@
         <v>31</v>
       </c>
       <c r="G14" s="4"/>
-      <c r="H14" s="13"/>
+      <c r="H14" s="8"/>
       <c r="I14" s="6"/>
       <c r="J14" s="6"/>
     </row>
@@ -1280,10 +1308,10 @@
       <c r="A16" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C16" s="11" t="s">
         <v>32</v>
       </c>
       <c r="D16" s="3">
@@ -1296,14 +1324,14 @@
         <v>67</v>
       </c>
       <c r="G16" s="4"/>
-      <c r="H16" s="12"/>
+      <c r="H16" s="7"/>
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:10" ht="21.75" thickBot="1">
       <c r="A17" s="6"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="10"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="12"/>
       <c r="D17" s="3">
         <v>2</v>
       </c>
@@ -1314,14 +1342,14 @@
         <v>23</v>
       </c>
       <c r="G17" s="4"/>
-      <c r="H17" s="13"/>
+      <c r="H17" s="8"/>
       <c r="I17" s="6"/>
       <c r="J17" s="6"/>
     </row>
     <row r="18" spans="1:10" ht="21.75" thickBot="1">
       <c r="A18" s="6"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="10"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="12"/>
       <c r="D18" s="3">
         <v>3</v>
       </c>
@@ -1332,14 +1360,14 @@
         <v>19</v>
       </c>
       <c r="G18" s="4"/>
-      <c r="H18" s="13"/>
+      <c r="H18" s="8"/>
       <c r="I18" s="6"/>
       <c r="J18" s="6"/>
     </row>
     <row r="19" spans="1:10" ht="42.75" thickBot="1">
       <c r="A19" s="6"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="10"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="12"/>
       <c r="D19" s="3">
         <v>4</v>
       </c>
@@ -1350,14 +1378,14 @@
         <v>24</v>
       </c>
       <c r="G19" s="4"/>
-      <c r="H19" s="13"/>
+      <c r="H19" s="8"/>
       <c r="I19" s="6"/>
       <c r="J19" s="6"/>
     </row>
     <row r="20" spans="1:10" ht="32.25" thickBot="1">
       <c r="A20" s="6"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="10"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="12"/>
       <c r="D20" s="3">
         <v>5</v>
       </c>
@@ -1368,14 +1396,14 @@
         <v>34</v>
       </c>
       <c r="G20" s="4"/>
-      <c r="H20" s="13"/>
+      <c r="H20" s="8"/>
       <c r="I20" s="6"/>
       <c r="J20" s="6"/>
     </row>
     <row r="21" spans="1:10" ht="32.25" thickBot="1">
       <c r="A21" s="6"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="10"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="12"/>
       <c r="D21" s="3">
         <v>6</v>
       </c>
@@ -1386,14 +1414,14 @@
         <v>35</v>
       </c>
       <c r="G21" s="4"/>
-      <c r="H21" s="13"/>
+      <c r="H21" s="8"/>
       <c r="I21" s="6"/>
       <c r="J21" s="6"/>
     </row>
     <row r="22" spans="1:10" ht="42.75" thickBot="1">
       <c r="A22" s="6"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="10"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="12"/>
       <c r="D22" s="3">
         <v>7</v>
       </c>
@@ -1404,7 +1432,7 @@
         <v>37</v>
       </c>
       <c r="G22" s="4"/>
-      <c r="H22" s="13"/>
+      <c r="H22" s="8"/>
       <c r="I22" s="6"/>
       <c r="J22" s="6"/>
     </row>
@@ -1424,10 +1452,10 @@
       <c r="A24" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="B24" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="C24" s="9" t="s">
+      <c r="C24" s="11" t="s">
         <v>40</v>
       </c>
       <c r="D24" s="3">
@@ -1440,14 +1468,14 @@
         <v>67</v>
       </c>
       <c r="G24" s="4"/>
-      <c r="H24" s="12"/>
+      <c r="H24" s="7"/>
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
     </row>
     <row r="25" spans="1:10" ht="21.75" thickBot="1">
       <c r="A25" s="6"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="10"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="12"/>
       <c r="D25" s="3">
         <v>2</v>
       </c>
@@ -1458,14 +1486,14 @@
         <v>23</v>
       </c>
       <c r="G25" s="4"/>
-      <c r="H25" s="13"/>
+      <c r="H25" s="8"/>
       <c r="I25" s="6"/>
       <c r="J25" s="6"/>
     </row>
     <row r="26" spans="1:10" ht="21.75" thickBot="1">
       <c r="A26" s="6"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="10"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="12"/>
       <c r="D26" s="3">
         <v>3</v>
       </c>
@@ -1476,14 +1504,14 @@
         <v>19</v>
       </c>
       <c r="G26" s="4"/>
-      <c r="H26" s="13"/>
+      <c r="H26" s="8"/>
       <c r="I26" s="6"/>
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="42.75" thickBot="1">
       <c r="A27" s="6"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="10"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="12"/>
       <c r="D27" s="3">
         <v>4</v>
       </c>
@@ -1494,14 +1522,14 @@
         <v>24</v>
       </c>
       <c r="G27" s="4"/>
-      <c r="H27" s="13"/>
+      <c r="H27" s="8"/>
       <c r="I27" s="6"/>
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="21.75" thickBot="1">
       <c r="A28" s="6"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="10"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="12"/>
       <c r="D28" s="3">
         <v>5</v>
       </c>
@@ -1512,14 +1540,14 @@
         <v>25</v>
       </c>
       <c r="G28" s="4"/>
-      <c r="H28" s="13"/>
+      <c r="H28" s="8"/>
       <c r="I28" s="6"/>
       <c r="J28" s="6"/>
     </row>
     <row r="29" spans="1:10" ht="32.25" thickBot="1">
       <c r="A29" s="6"/>
-      <c r="B29" s="8"/>
-      <c r="C29" s="10"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="12"/>
       <c r="D29" s="3">
         <v>6</v>
       </c>
@@ -1530,7 +1558,7 @@
         <v>39</v>
       </c>
       <c r="G29" s="4"/>
-      <c r="H29" s="13"/>
+      <c r="H29" s="8"/>
       <c r="I29" s="6"/>
       <c r="J29" s="6"/>
     </row>
@@ -1550,10 +1578,10 @@
       <c r="A31" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B31" s="7" t="s">
+      <c r="B31" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="C31" s="9" t="s">
+      <c r="C31" s="11" t="s">
         <v>41</v>
       </c>
       <c r="D31" s="3">
@@ -1566,14 +1594,14 @@
         <v>67</v>
       </c>
       <c r="G31" s="4"/>
-      <c r="H31" s="12"/>
+      <c r="H31" s="7"/>
       <c r="I31" s="5"/>
       <c r="J31" s="5"/>
     </row>
     <row r="32" spans="1:10" ht="21.75" thickBot="1">
       <c r="A32" s="6"/>
-      <c r="B32" s="8"/>
-      <c r="C32" s="10"/>
+      <c r="B32" s="10"/>
+      <c r="C32" s="12"/>
       <c r="D32" s="3">
         <v>2</v>
       </c>
@@ -1584,14 +1612,14 @@
         <v>23</v>
       </c>
       <c r="G32" s="4"/>
-      <c r="H32" s="13"/>
+      <c r="H32" s="8"/>
       <c r="I32" s="6"/>
       <c r="J32" s="6"/>
     </row>
     <row r="33" spans="1:10" ht="21.75" thickBot="1">
       <c r="A33" s="6"/>
-      <c r="B33" s="8"/>
-      <c r="C33" s="10"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="12"/>
       <c r="D33" s="3">
         <v>3</v>
       </c>
@@ -1602,14 +1630,14 @@
         <v>19</v>
       </c>
       <c r="G33" s="4"/>
-      <c r="H33" s="13"/>
+      <c r="H33" s="8"/>
       <c r="I33" s="6"/>
       <c r="J33" s="6"/>
     </row>
     <row r="34" spans="1:10" ht="42.75" thickBot="1">
       <c r="A34" s="6"/>
-      <c r="B34" s="8"/>
-      <c r="C34" s="10"/>
+      <c r="B34" s="10"/>
+      <c r="C34" s="12"/>
       <c r="D34" s="3">
         <v>4</v>
       </c>
@@ -1620,14 +1648,14 @@
         <v>24</v>
       </c>
       <c r="G34" s="4"/>
-      <c r="H34" s="13"/>
+      <c r="H34" s="8"/>
       <c r="I34" s="6"/>
       <c r="J34" s="6"/>
     </row>
     <row r="35" spans="1:10" ht="32.25" thickBot="1">
       <c r="A35" s="6"/>
-      <c r="B35" s="8"/>
-      <c r="C35" s="10"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="12"/>
       <c r="D35" s="3">
         <v>5</v>
       </c>
@@ -1638,14 +1666,14 @@
         <v>34</v>
       </c>
       <c r="G35" s="4"/>
-      <c r="H35" s="13"/>
+      <c r="H35" s="8"/>
       <c r="I35" s="6"/>
       <c r="J35" s="6"/>
     </row>
     <row r="36" spans="1:10" ht="32.25" thickBot="1">
       <c r="A36" s="6"/>
-      <c r="B36" s="8"/>
-      <c r="C36" s="10"/>
+      <c r="B36" s="10"/>
+      <c r="C36" s="12"/>
       <c r="D36" s="3">
         <v>6</v>
       </c>
@@ -1656,14 +1684,14 @@
         <v>35</v>
       </c>
       <c r="G36" s="4"/>
-      <c r="H36" s="13"/>
+      <c r="H36" s="8"/>
       <c r="I36" s="6"/>
       <c r="J36" s="6"/>
     </row>
     <row r="37" spans="1:10" ht="42.75" thickBot="1">
       <c r="A37" s="6"/>
-      <c r="B37" s="8"/>
-      <c r="C37" s="10"/>
+      <c r="B37" s="10"/>
+      <c r="C37" s="12"/>
       <c r="D37" s="3">
         <v>7</v>
       </c>
@@ -1674,7 +1702,7 @@
         <v>43</v>
       </c>
       <c r="G37" s="4"/>
-      <c r="H37" s="13"/>
+      <c r="H37" s="8"/>
       <c r="I37" s="6"/>
       <c r="J37" s="6"/>
     </row>
@@ -1692,36 +1720,36 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="A31:A37"/>
+    <mergeCell ref="B31:B37"/>
+    <mergeCell ref="C31:C37"/>
+    <mergeCell ref="B9:B14"/>
+    <mergeCell ref="C9:C14"/>
+    <mergeCell ref="B2:B7"/>
+    <mergeCell ref="H31:H37"/>
+    <mergeCell ref="I31:I37"/>
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="C2:C7"/>
+    <mergeCell ref="I16:I22"/>
+    <mergeCell ref="A24:A29"/>
+    <mergeCell ref="B24:B29"/>
+    <mergeCell ref="C24:C29"/>
+    <mergeCell ref="H24:H29"/>
+    <mergeCell ref="I24:I29"/>
+    <mergeCell ref="A9:A14"/>
+    <mergeCell ref="A16:A22"/>
+    <mergeCell ref="B16:B22"/>
+    <mergeCell ref="C16:C22"/>
+    <mergeCell ref="H16:H22"/>
     <mergeCell ref="J31:J37"/>
     <mergeCell ref="H9:H14"/>
     <mergeCell ref="I9:I14"/>
     <mergeCell ref="J9:J14"/>
     <mergeCell ref="H2:H7"/>
     <mergeCell ref="I2:I7"/>
-    <mergeCell ref="B2:B7"/>
-    <mergeCell ref="H31:H37"/>
-    <mergeCell ref="I31:I37"/>
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="C2:C7"/>
-    <mergeCell ref="I16:I22"/>
     <mergeCell ref="J16:J22"/>
-    <mergeCell ref="A24:A29"/>
-    <mergeCell ref="B24:B29"/>
-    <mergeCell ref="C24:C29"/>
-    <mergeCell ref="H24:H29"/>
-    <mergeCell ref="I24:I29"/>
     <mergeCell ref="J24:J29"/>
-    <mergeCell ref="A9:A14"/>
-    <mergeCell ref="A16:A22"/>
-    <mergeCell ref="B16:B22"/>
-    <mergeCell ref="C16:C22"/>
-    <mergeCell ref="H16:H22"/>
     <mergeCell ref="J2:J7"/>
-    <mergeCell ref="A31:A37"/>
-    <mergeCell ref="B31:B37"/>
-    <mergeCell ref="C31:C37"/>
-    <mergeCell ref="B9:B14"/>
-    <mergeCell ref="C9:C14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1798,10 +1826,10 @@
       <c r="A2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="11" t="s">
         <v>45</v>
       </c>
       <c r="D2" s="3">
@@ -1814,7 +1842,7 @@
         <v>67</v>
       </c>
       <c r="G2" s="4"/>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="7" t="s">
         <v>9</v>
       </c>
       <c r="I2" s="5"/>
@@ -1822,8 +1850,8 @@
     </row>
     <row r="3" spans="1:10" ht="42.75" customHeight="1" thickBot="1">
       <c r="A3" s="6"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="10"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="12"/>
       <c r="D3" s="3">
         <v>2</v>
       </c>
@@ -1834,14 +1862,14 @@
         <v>23</v>
       </c>
       <c r="G3" s="4"/>
-      <c r="H3" s="13"/>
+      <c r="H3" s="8"/>
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
     </row>
     <row r="4" spans="1:10" ht="21.75" thickBot="1">
       <c r="A4" s="6"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="10"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="12"/>
       <c r="D4" s="3">
         <v>3</v>
       </c>
@@ -1852,14 +1880,14 @@
         <v>19</v>
       </c>
       <c r="G4" s="4"/>
-      <c r="H4" s="13"/>
+      <c r="H4" s="8"/>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
     </row>
     <row r="5" spans="1:10" ht="42.75" thickBot="1">
       <c r="A5" s="6"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="10"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="12"/>
       <c r="D5" s="3">
         <v>4</v>
       </c>
@@ -1870,14 +1898,14 @@
         <v>24</v>
       </c>
       <c r="G5" s="4"/>
-      <c r="H5" s="13"/>
+      <c r="H5" s="8"/>
       <c r="I5" s="6"/>
       <c r="J5" s="6"/>
     </row>
     <row r="6" spans="1:10" ht="21.75" thickBot="1">
       <c r="A6" s="6"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="10"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="12"/>
       <c r="D6" s="3">
         <v>5</v>
       </c>
@@ -1888,14 +1916,14 @@
         <v>48</v>
       </c>
       <c r="G6" s="4"/>
-      <c r="H6" s="13"/>
+      <c r="H6" s="8"/>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
     </row>
     <row r="7" spans="1:10" ht="32.25" thickBot="1">
       <c r="A7" s="6"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="10"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="12"/>
       <c r="D7" s="3">
         <v>6</v>
       </c>
@@ -1906,7 +1934,7 @@
         <v>50</v>
       </c>
       <c r="G7" s="4"/>
-      <c r="H7" s="13"/>
+      <c r="H7" s="8"/>
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
     </row>
@@ -1926,10 +1954,10 @@
       <c r="A9" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="11" t="s">
         <v>52</v>
       </c>
       <c r="D9" s="3">
@@ -1942,7 +1970,7 @@
         <v>67</v>
       </c>
       <c r="G9" s="4"/>
-      <c r="H9" s="12" t="s">
+      <c r="H9" s="7" t="s">
         <v>9</v>
       </c>
       <c r="I9" s="5"/>
@@ -1950,8 +1978,8 @@
     </row>
     <row r="10" spans="1:10" ht="21.75" thickBot="1">
       <c r="A10" s="6"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="10"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="12"/>
       <c r="D10" s="3">
         <v>2</v>
       </c>
@@ -1962,14 +1990,14 @@
         <v>23</v>
       </c>
       <c r="G10" s="4"/>
-      <c r="H10" s="13"/>
+      <c r="H10" s="8"/>
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
     </row>
     <row r="11" spans="1:10" ht="21.75" thickBot="1">
       <c r="A11" s="6"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="10"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="12"/>
       <c r="D11" s="3">
         <v>3</v>
       </c>
@@ -1980,14 +2008,14 @@
         <v>19</v>
       </c>
       <c r="G11" s="4"/>
-      <c r="H11" s="13"/>
+      <c r="H11" s="8"/>
       <c r="I11" s="6"/>
       <c r="J11" s="6"/>
     </row>
     <row r="12" spans="1:10" ht="42.75" thickBot="1">
       <c r="A12" s="6"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="10"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="12"/>
       <c r="D12" s="3">
         <v>4</v>
       </c>
@@ -1998,14 +2026,14 @@
         <v>24</v>
       </c>
       <c r="G12" s="4"/>
-      <c r="H12" s="13"/>
+      <c r="H12" s="8"/>
       <c r="I12" s="6"/>
       <c r="J12" s="6"/>
     </row>
     <row r="13" spans="1:10" ht="21.75" thickBot="1">
       <c r="A13" s="6"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="10"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="12"/>
       <c r="D13" s="3">
         <v>5</v>
       </c>
@@ -2016,14 +2044,14 @@
         <v>48</v>
       </c>
       <c r="G13" s="4"/>
-      <c r="H13" s="13"/>
+      <c r="H13" s="8"/>
       <c r="I13" s="6"/>
       <c r="J13" s="6"/>
     </row>
     <row r="14" spans="1:10" ht="42.75" thickBot="1">
       <c r="A14" s="6"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="10"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="12"/>
       <c r="D14" s="3">
         <v>6</v>
       </c>
@@ -2034,7 +2062,7 @@
         <v>54</v>
       </c>
       <c r="G14" s="4"/>
-      <c r="H14" s="13"/>
+      <c r="H14" s="8"/>
       <c r="I14" s="6"/>
       <c r="J14" s="6"/>
     </row>
@@ -2092,8 +2120,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29:F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2140,10 +2168,10 @@
       <c r="A2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="11" t="s">
         <v>60</v>
       </c>
       <c r="D2" s="3">
@@ -2156,7 +2184,7 @@
         <v>67</v>
       </c>
       <c r="G2" s="4"/>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="7" t="s">
         <v>9</v>
       </c>
       <c r="I2" s="5"/>
@@ -2164,8 +2192,8 @@
     </row>
     <row r="3" spans="1:10" ht="32.25" thickBot="1">
       <c r="A3" s="6"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="10"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="12"/>
       <c r="D3" s="3">
         <v>2</v>
       </c>
@@ -2176,14 +2204,14 @@
         <v>57</v>
       </c>
       <c r="G3" s="4"/>
-      <c r="H3" s="13"/>
+      <c r="H3" s="8"/>
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
     </row>
     <row r="4" spans="1:10" ht="21.75" thickBot="1">
       <c r="A4" s="6"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="10"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="12"/>
       <c r="D4" s="3">
         <v>3</v>
       </c>
@@ -2194,14 +2222,14 @@
         <v>19</v>
       </c>
       <c r="G4" s="4"/>
-      <c r="H4" s="13"/>
+      <c r="H4" s="8"/>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
     </row>
     <row r="5" spans="1:10" ht="53.25" thickBot="1">
       <c r="A5" s="6"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="10"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="12"/>
       <c r="D5" s="3">
         <v>4</v>
       </c>
@@ -2212,14 +2240,14 @@
         <v>73</v>
       </c>
       <c r="G5" s="4"/>
-      <c r="H5" s="13"/>
+      <c r="H5" s="8"/>
       <c r="I5" s="6"/>
       <c r="J5" s="6"/>
     </row>
     <row r="6" spans="1:10" ht="21.75" thickBot="1">
       <c r="A6" s="6"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="10"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="12"/>
       <c r="D6" s="3">
         <v>5</v>
       </c>
@@ -2230,7 +2258,7 @@
         <v>72</v>
       </c>
       <c r="G6" s="4"/>
-      <c r="H6" s="13"/>
+      <c r="H6" s="8"/>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
     </row>
@@ -2250,10 +2278,10 @@
       <c r="A8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="11" t="s">
         <v>74</v>
       </c>
       <c r="D8" s="3">
@@ -2266,7 +2294,7 @@
         <v>67</v>
       </c>
       <c r="G8" s="4"/>
-      <c r="H8" s="12" t="s">
+      <c r="H8" s="7" t="s">
         <v>9</v>
       </c>
       <c r="I8" s="5"/>
@@ -2274,8 +2302,8 @@
     </row>
     <row r="9" spans="1:10" ht="32.25" thickBot="1">
       <c r="A9" s="6"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="10"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="12"/>
       <c r="D9" s="3">
         <v>2</v>
       </c>
@@ -2286,14 +2314,14 @@
         <v>23</v>
       </c>
       <c r="G9" s="4"/>
-      <c r="H9" s="13"/>
+      <c r="H9" s="8"/>
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
     </row>
     <row r="10" spans="1:10" ht="21.75" thickBot="1">
       <c r="A10" s="6"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="10"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="12"/>
       <c r="D10" s="3">
         <v>3</v>
       </c>
@@ -2304,14 +2332,14 @@
         <v>19</v>
       </c>
       <c r="G10" s="4"/>
-      <c r="H10" s="13"/>
+      <c r="H10" s="8"/>
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
     </row>
     <row r="11" spans="1:10" ht="42.75" thickBot="1">
       <c r="A11" s="6"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="10"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="12"/>
       <c r="D11" s="3">
         <v>4</v>
       </c>
@@ -2322,7 +2350,7 @@
         <v>76</v>
       </c>
       <c r="G11" s="4"/>
-      <c r="H11" s="13"/>
+      <c r="H11" s="8"/>
       <c r="I11" s="6"/>
       <c r="J11" s="6"/>
     </row>
@@ -2342,10 +2370,10 @@
       <c r="A13" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="11" t="s">
         <v>79</v>
       </c>
       <c r="D13" s="3">
@@ -2358,7 +2386,7 @@
         <v>67</v>
       </c>
       <c r="G13" s="4"/>
-      <c r="H13" s="12" t="s">
+      <c r="H13" s="7" t="s">
         <v>9</v>
       </c>
       <c r="I13" s="5"/>
@@ -2366,8 +2394,8 @@
     </row>
     <row r="14" spans="1:10" ht="32.25" thickBot="1">
       <c r="A14" s="6"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="10"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="12"/>
       <c r="D14" s="3">
         <v>2</v>
       </c>
@@ -2378,14 +2406,14 @@
         <v>57</v>
       </c>
       <c r="G14" s="4"/>
-      <c r="H14" s="13"/>
+      <c r="H14" s="8"/>
       <c r="I14" s="6"/>
       <c r="J14" s="6"/>
     </row>
     <row r="15" spans="1:10" ht="21.75" thickBot="1">
       <c r="A15" s="6"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="10"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="12"/>
       <c r="D15" s="3">
         <v>3</v>
       </c>
@@ -2396,14 +2424,14 @@
         <v>19</v>
       </c>
       <c r="G15" s="4"/>
-      <c r="H15" s="13"/>
+      <c r="H15" s="8"/>
       <c r="I15" s="6"/>
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10" ht="63.75" thickBot="1">
       <c r="A16" s="6"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="10"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="12"/>
       <c r="D16" s="3">
         <v>4</v>
       </c>
@@ -2414,7 +2442,7 @@
         <v>80</v>
       </c>
       <c r="G16" s="4"/>
-      <c r="H16" s="13"/>
+      <c r="H16" s="8"/>
       <c r="I16" s="6"/>
       <c r="J16" s="6"/>
     </row>
@@ -2434,10 +2462,10 @@
       <c r="A18" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="C18" s="11" t="s">
         <v>91</v>
       </c>
       <c r="D18" s="3">
@@ -2450,7 +2478,7 @@
         <v>67</v>
       </c>
       <c r="G18" s="4"/>
-      <c r="H18" s="12" t="s">
+      <c r="H18" s="7" t="s">
         <v>9</v>
       </c>
       <c r="I18" s="5"/>
@@ -2458,8 +2486,8 @@
     </row>
     <row r="19" spans="1:10" ht="32.25" thickBot="1">
       <c r="A19" s="6"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="10"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="12"/>
       <c r="D19" s="3">
         <v>2</v>
       </c>
@@ -2470,14 +2498,14 @@
         <v>57</v>
       </c>
       <c r="G19" s="4"/>
-      <c r="H19" s="13"/>
+      <c r="H19" s="8"/>
       <c r="I19" s="6"/>
       <c r="J19" s="6"/>
     </row>
     <row r="20" spans="1:10" ht="21.75" thickBot="1">
       <c r="A20" s="6"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="10"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="12"/>
       <c r="D20" s="3">
         <v>3</v>
       </c>
@@ -2488,14 +2516,14 @@
         <v>19</v>
       </c>
       <c r="G20" s="4"/>
-      <c r="H20" s="13"/>
+      <c r="H20" s="8"/>
       <c r="I20" s="6"/>
       <c r="J20" s="6"/>
     </row>
     <row r="21" spans="1:10" ht="21.75" thickBot="1">
       <c r="A21" s="6"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="10"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="12"/>
       <c r="D21" s="3">
         <v>4</v>
       </c>
@@ -2506,14 +2534,14 @@
         <v>83</v>
       </c>
       <c r="G21" s="4"/>
-      <c r="H21" s="13"/>
+      <c r="H21" s="8"/>
       <c r="I21" s="6"/>
       <c r="J21" s="6"/>
     </row>
     <row r="22" spans="1:10" ht="95.25" thickBot="1">
       <c r="A22" s="6"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="10"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="12"/>
       <c r="D22" s="3">
         <v>5</v>
       </c>
@@ -2524,14 +2552,14 @@
         <v>85</v>
       </c>
       <c r="G22" s="4"/>
-      <c r="H22" s="13"/>
+      <c r="H22" s="8"/>
       <c r="I22" s="6"/>
       <c r="J22" s="6"/>
     </row>
     <row r="23" spans="1:10" ht="21.75" thickBot="1">
       <c r="A23" s="6"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="10"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="12"/>
       <c r="D23" s="3">
         <v>6</v>
       </c>
@@ -2542,14 +2570,14 @@
         <v>87</v>
       </c>
       <c r="G23" s="4"/>
-      <c r="H23" s="13"/>
+      <c r="H23" s="8"/>
       <c r="I23" s="6"/>
       <c r="J23" s="6"/>
     </row>
     <row r="24" spans="1:10" ht="32.25" thickBot="1">
       <c r="A24" s="6"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="10"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="12"/>
       <c r="D24" s="3">
         <v>7</v>
       </c>
@@ -2558,14 +2586,14 @@
       </c>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
-      <c r="H24" s="13"/>
+      <c r="H24" s="8"/>
       <c r="I24" s="6"/>
       <c r="J24" s="6"/>
     </row>
     <row r="25" spans="1:10" ht="21.75" thickBot="1">
       <c r="A25" s="6"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="10"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="12"/>
       <c r="D25" s="3">
         <v>8</v>
       </c>
@@ -2574,14 +2602,14 @@
       </c>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
-      <c r="H25" s="13"/>
+      <c r="H25" s="8"/>
       <c r="I25" s="6"/>
       <c r="J25" s="6"/>
     </row>
     <row r="26" spans="1:10" ht="42.75" thickBot="1">
       <c r="A26" s="6"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="10"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="12"/>
       <c r="D26" s="3">
         <v>9</v>
       </c>
@@ -2590,14 +2618,14 @@
       </c>
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
-      <c r="H26" s="13"/>
+      <c r="H26" s="8"/>
       <c r="I26" s="6"/>
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="21.75" thickBot="1">
       <c r="A27" s="6"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="10"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="12"/>
       <c r="D27" s="3">
         <v>10</v>
       </c>
@@ -2608,7 +2636,7 @@
         <v>93</v>
       </c>
       <c r="G27" s="4"/>
-      <c r="H27" s="13"/>
+      <c r="H27" s="8"/>
       <c r="I27" s="6"/>
       <c r="J27" s="6"/>
     </row>
@@ -2628,10 +2656,10 @@
       <c r="A29" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B29" s="7" t="s">
+      <c r="B29" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="C29" s="9" t="s">
+      <c r="C29" s="11" t="s">
         <v>120</v>
       </c>
       <c r="D29" s="3">
@@ -2644,7 +2672,7 @@
         <v>67</v>
       </c>
       <c r="G29" s="4"/>
-      <c r="H29" s="12" t="s">
+      <c r="H29" s="7" t="s">
         <v>9</v>
       </c>
       <c r="I29" s="5"/>
@@ -2652,8 +2680,8 @@
     </row>
     <row r="30" spans="1:10" ht="32.25" thickBot="1">
       <c r="A30" s="6"/>
-      <c r="B30" s="8"/>
-      <c r="C30" s="10"/>
+      <c r="B30" s="10"/>
+      <c r="C30" s="12"/>
       <c r="D30" s="3">
         <v>2</v>
       </c>
@@ -2664,14 +2692,14 @@
         <v>57</v>
       </c>
       <c r="G30" s="4"/>
-      <c r="H30" s="13"/>
+      <c r="H30" s="8"/>
       <c r="I30" s="6"/>
       <c r="J30" s="6"/>
     </row>
     <row r="31" spans="1:10" ht="21.75" thickBot="1">
       <c r="A31" s="6"/>
-      <c r="B31" s="8"/>
-      <c r="C31" s="10"/>
+      <c r="B31" s="10"/>
+      <c r="C31" s="12"/>
       <c r="D31" s="3">
         <v>3</v>
       </c>
@@ -2682,14 +2710,14 @@
         <v>19</v>
       </c>
       <c r="G31" s="4"/>
-      <c r="H31" s="13"/>
+      <c r="H31" s="8"/>
       <c r="I31" s="6"/>
       <c r="J31" s="6"/>
     </row>
     <row r="32" spans="1:10" ht="21.75" thickBot="1">
       <c r="A32" s="6"/>
-      <c r="B32" s="8"/>
-      <c r="C32" s="10"/>
+      <c r="B32" s="10"/>
+      <c r="C32" s="12"/>
       <c r="D32" s="3">
         <v>4</v>
       </c>
@@ -2700,14 +2728,14 @@
         <v>83</v>
       </c>
       <c r="G32" s="4"/>
-      <c r="H32" s="13"/>
+      <c r="H32" s="8"/>
       <c r="I32" s="6"/>
       <c r="J32" s="6"/>
     </row>
     <row r="33" spans="1:10" ht="95.25" thickBot="1">
       <c r="A33" s="6"/>
-      <c r="B33" s="8"/>
-      <c r="C33" s="10"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="12"/>
       <c r="D33" s="3">
         <v>5</v>
       </c>
@@ -2718,14 +2746,14 @@
         <v>85</v>
       </c>
       <c r="G33" s="4"/>
-      <c r="H33" s="13"/>
+      <c r="H33" s="8"/>
       <c r="I33" s="6"/>
       <c r="J33" s="6"/>
     </row>
     <row r="34" spans="1:10" ht="21.75" thickBot="1">
       <c r="A34" s="6"/>
-      <c r="B34" s="8"/>
-      <c r="C34" s="10"/>
+      <c r="B34" s="10"/>
+      <c r="C34" s="12"/>
       <c r="D34" s="3">
         <v>6</v>
       </c>
@@ -2736,14 +2764,14 @@
         <v>87</v>
       </c>
       <c r="G34" s="4"/>
-      <c r="H34" s="13"/>
+      <c r="H34" s="8"/>
       <c r="I34" s="6"/>
       <c r="J34" s="6"/>
     </row>
     <row r="35" spans="1:10" ht="15.75" thickBot="1">
       <c r="A35" s="6"/>
-      <c r="B35" s="8"/>
-      <c r="C35" s="10"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="12"/>
       <c r="D35" s="3">
         <v>7</v>
       </c>
@@ -2754,14 +2782,14 @@
         <v>111</v>
       </c>
       <c r="G35" s="4"/>
-      <c r="H35" s="13"/>
+      <c r="H35" s="8"/>
       <c r="I35" s="6"/>
       <c r="J35" s="6"/>
     </row>
     <row r="36" spans="1:10" ht="21.75" thickBot="1">
       <c r="A36" s="6"/>
-      <c r="B36" s="8"/>
-      <c r="C36" s="10"/>
+      <c r="B36" s="10"/>
+      <c r="C36" s="12"/>
       <c r="D36" s="3">
         <v>8</v>
       </c>
@@ -2770,14 +2798,14 @@
       </c>
       <c r="F36" s="4"/>
       <c r="G36" s="4"/>
-      <c r="H36" s="13"/>
+      <c r="H36" s="8"/>
       <c r="I36" s="6"/>
       <c r="J36" s="6"/>
     </row>
     <row r="37" spans="1:10" ht="42.75" thickBot="1">
       <c r="A37" s="6"/>
-      <c r="B37" s="8"/>
-      <c r="C37" s="10"/>
+      <c r="B37" s="10"/>
+      <c r="C37" s="12"/>
       <c r="D37" s="3">
         <v>9</v>
       </c>
@@ -2786,14 +2814,14 @@
       </c>
       <c r="F37" s="4"/>
       <c r="G37" s="4"/>
-      <c r="H37" s="13"/>
+      <c r="H37" s="8"/>
       <c r="I37" s="6"/>
       <c r="J37" s="6"/>
     </row>
     <row r="38" spans="1:10" ht="21.75" thickBot="1">
       <c r="A38" s="6"/>
-      <c r="B38" s="8"/>
-      <c r="C38" s="10"/>
+      <c r="B38" s="10"/>
+      <c r="C38" s="12"/>
       <c r="D38" s="3">
         <v>10</v>
       </c>
@@ -2804,7 +2832,7 @@
         <v>93</v>
       </c>
       <c r="G38" s="4"/>
-      <c r="H38" s="13"/>
+      <c r="H38" s="8"/>
       <c r="I38" s="6"/>
       <c r="J38" s="6"/>
     </row>
@@ -2822,12 +2850,18 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="J29:J38"/>
-    <mergeCell ref="A29:A38"/>
-    <mergeCell ref="B29:B38"/>
-    <mergeCell ref="C29:C38"/>
-    <mergeCell ref="H29:H38"/>
-    <mergeCell ref="I29:I38"/>
+    <mergeCell ref="A18:A27"/>
+    <mergeCell ref="J18:J27"/>
+    <mergeCell ref="I18:I27"/>
+    <mergeCell ref="H18:H27"/>
+    <mergeCell ref="C18:C27"/>
+    <mergeCell ref="B18:B27"/>
+    <mergeCell ref="J13:J16"/>
+    <mergeCell ref="A13:A16"/>
+    <mergeCell ref="B13:B16"/>
+    <mergeCell ref="C13:C16"/>
+    <mergeCell ref="H13:H16"/>
+    <mergeCell ref="I13:I16"/>
     <mergeCell ref="J2:J6"/>
     <mergeCell ref="A8:A11"/>
     <mergeCell ref="B8:B11"/>
@@ -2840,18 +2874,12 @@
     <mergeCell ref="C2:C6"/>
     <mergeCell ref="H2:H6"/>
     <mergeCell ref="I2:I6"/>
-    <mergeCell ref="J13:J16"/>
-    <mergeCell ref="A13:A16"/>
-    <mergeCell ref="B13:B16"/>
-    <mergeCell ref="C13:C16"/>
-    <mergeCell ref="H13:H16"/>
-    <mergeCell ref="I13:I16"/>
-    <mergeCell ref="A18:A27"/>
-    <mergeCell ref="J18:J27"/>
-    <mergeCell ref="I18:I27"/>
-    <mergeCell ref="H18:H27"/>
-    <mergeCell ref="C18:C27"/>
-    <mergeCell ref="B18:B27"/>
+    <mergeCell ref="J29:J38"/>
+    <mergeCell ref="A29:A38"/>
+    <mergeCell ref="B29:B38"/>
+    <mergeCell ref="C29:C38"/>
+    <mergeCell ref="H29:H38"/>
+    <mergeCell ref="I29:I38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2880,7 +2908,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
+    <sheetView topLeftCell="A40" workbookViewId="0">
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
@@ -2926,10 +2954,10 @@
       <c r="A2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="11" t="s">
         <v>94</v>
       </c>
       <c r="D2" s="3">
@@ -2942,7 +2970,7 @@
         <v>67</v>
       </c>
       <c r="G2" s="4"/>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="7" t="s">
         <v>9</v>
       </c>
       <c r="I2" s="5"/>
@@ -2950,8 +2978,8 @@
     </row>
     <row r="3" spans="1:10" ht="32.25" thickBot="1">
       <c r="A3" s="6"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="10"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="12"/>
       <c r="D3" s="3">
         <v>2</v>
       </c>
@@ -2962,14 +2990,14 @@
         <v>23</v>
       </c>
       <c r="G3" s="4"/>
-      <c r="H3" s="13"/>
+      <c r="H3" s="8"/>
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
     </row>
     <row r="4" spans="1:10" ht="21.75" thickBot="1">
       <c r="A4" s="6"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="10"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="12"/>
       <c r="D4" s="3">
         <v>3</v>
       </c>
@@ -2980,14 +3008,14 @@
         <v>19</v>
       </c>
       <c r="G4" s="4"/>
-      <c r="H4" s="13"/>
+      <c r="H4" s="8"/>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
     </row>
     <row r="5" spans="1:10" ht="42.75" thickBot="1">
       <c r="A5" s="6"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="10"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="12"/>
       <c r="D5" s="3">
         <v>4</v>
       </c>
@@ -2998,14 +3026,14 @@
         <v>24</v>
       </c>
       <c r="G5" s="4"/>
-      <c r="H5" s="13"/>
+      <c r="H5" s="8"/>
       <c r="I5" s="6"/>
       <c r="J5" s="6"/>
     </row>
     <row r="6" spans="1:10" ht="84.75" thickBot="1">
       <c r="A6" s="6"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="10"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="12"/>
       <c r="D6" s="3">
         <v>5</v>
       </c>
@@ -3016,14 +3044,14 @@
         <v>98</v>
       </c>
       <c r="G6" s="4"/>
-      <c r="H6" s="13"/>
+      <c r="H6" s="8"/>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
     </row>
     <row r="7" spans="1:10" ht="32.25" thickBot="1">
       <c r="A7" s="6"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="10"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="12"/>
       <c r="D7" s="3">
         <v>6</v>
       </c>
@@ -3032,14 +3060,14 @@
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
-      <c r="H7" s="13"/>
+      <c r="H7" s="8"/>
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
     </row>
     <row r="8" spans="1:10" ht="21.75" thickBot="1">
       <c r="A8" s="6"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="10"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="12"/>
       <c r="D8" s="3">
         <v>7</v>
       </c>
@@ -3048,14 +3076,14 @@
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
-      <c r="H8" s="13"/>
+      <c r="H8" s="8"/>
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
     </row>
     <row r="9" spans="1:10" ht="32.25" thickBot="1">
       <c r="A9" s="6"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="10"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="12"/>
       <c r="D9" s="3">
         <v>8</v>
       </c>
@@ -3064,7 +3092,7 @@
       </c>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
-      <c r="H9" s="13"/>
+      <c r="H9" s="8"/>
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
     </row>
@@ -3084,10 +3112,10 @@
       <c r="A11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="11" t="s">
         <v>102</v>
       </c>
       <c r="D11" s="3">
@@ -3100,7 +3128,7 @@
         <v>67</v>
       </c>
       <c r="G11" s="4"/>
-      <c r="H11" s="12" t="s">
+      <c r="H11" s="7" t="s">
         <v>9</v>
       </c>
       <c r="I11" s="5"/>
@@ -3108,8 +3136,8 @@
     </row>
     <row r="12" spans="1:10" ht="32.25" thickBot="1">
       <c r="A12" s="6"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="10"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="12"/>
       <c r="D12" s="3">
         <v>2</v>
       </c>
@@ -3120,14 +3148,14 @@
         <v>23</v>
       </c>
       <c r="G12" s="4"/>
-      <c r="H12" s="13"/>
+      <c r="H12" s="8"/>
       <c r="I12" s="6"/>
       <c r="J12" s="6"/>
     </row>
     <row r="13" spans="1:10" ht="21.75" thickBot="1">
       <c r="A13" s="6"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="10"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="12"/>
       <c r="D13" s="3">
         <v>3</v>
       </c>
@@ -3138,14 +3166,14 @@
         <v>19</v>
       </c>
       <c r="G13" s="4"/>
-      <c r="H13" s="13"/>
+      <c r="H13" s="8"/>
       <c r="I13" s="6"/>
       <c r="J13" s="6"/>
     </row>
     <row r="14" spans="1:10" ht="42.75" thickBot="1">
       <c r="A14" s="6"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="10"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="12"/>
       <c r="D14" s="3">
         <v>4</v>
       </c>
@@ -3156,14 +3184,14 @@
         <v>24</v>
       </c>
       <c r="G14" s="4"/>
-      <c r="H14" s="13"/>
+      <c r="H14" s="8"/>
       <c r="I14" s="6"/>
       <c r="J14" s="6"/>
     </row>
     <row r="15" spans="1:10" ht="84.75" thickBot="1">
       <c r="A15" s="6"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="10"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="12"/>
       <c r="D15" s="3">
         <v>5</v>
       </c>
@@ -3174,14 +3202,14 @@
         <v>98</v>
       </c>
       <c r="G15" s="4"/>
-      <c r="H15" s="13"/>
+      <c r="H15" s="8"/>
       <c r="I15" s="6"/>
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10" ht="32.25" thickBot="1">
       <c r="A16" s="6"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="10"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="12"/>
       <c r="D16" s="3">
         <v>6</v>
       </c>
@@ -3190,14 +3218,14 @@
       </c>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
-      <c r="H16" s="13"/>
+      <c r="H16" s="8"/>
       <c r="I16" s="6"/>
       <c r="J16" s="6"/>
     </row>
     <row r="17" spans="1:10" ht="21.75" thickBot="1">
       <c r="A17" s="6"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="10"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="12"/>
       <c r="D17" s="3">
         <v>7</v>
       </c>
@@ -3206,14 +3234,14 @@
       </c>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
-      <c r="H17" s="13"/>
+      <c r="H17" s="8"/>
       <c r="I17" s="6"/>
       <c r="J17" s="6"/>
     </row>
     <row r="18" spans="1:10" ht="32.25" thickBot="1">
       <c r="A18" s="6"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="10"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="12"/>
       <c r="D18" s="3">
         <v>8</v>
       </c>
@@ -3222,14 +3250,14 @@
       </c>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
-      <c r="H18" s="13"/>
+      <c r="H18" s="8"/>
       <c r="I18" s="6"/>
       <c r="J18" s="6"/>
     </row>
     <row r="19" spans="1:10" ht="32.25" thickBot="1">
       <c r="A19" s="6"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="10"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="12"/>
       <c r="D19" s="3">
         <v>9</v>
       </c>
@@ -3240,14 +3268,14 @@
         <v>105</v>
       </c>
       <c r="G19" s="4"/>
-      <c r="H19" s="13"/>
+      <c r="H19" s="8"/>
       <c r="I19" s="6"/>
       <c r="J19" s="6"/>
     </row>
     <row r="20" spans="1:10" ht="42.75" thickBot="1">
       <c r="A20" s="6"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="10"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="12"/>
       <c r="D20" s="3">
         <v>10</v>
       </c>
@@ -3258,7 +3286,7 @@
         <v>118</v>
       </c>
       <c r="G20" s="4"/>
-      <c r="H20" s="13"/>
+      <c r="H20" s="8"/>
       <c r="I20" s="6"/>
       <c r="J20" s="6"/>
     </row>
@@ -3278,10 +3306,10 @@
       <c r="A22" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="B22" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C22" s="11" t="s">
         <v>114</v>
       </c>
       <c r="D22" s="3">
@@ -3294,7 +3322,7 @@
         <v>67</v>
       </c>
       <c r="G22" s="4"/>
-      <c r="H22" s="12" t="s">
+      <c r="H22" s="7" t="s">
         <v>9</v>
       </c>
       <c r="I22" s="5"/>
@@ -3302,8 +3330,8 @@
     </row>
     <row r="23" spans="1:10" ht="32.25" thickBot="1">
       <c r="A23" s="6"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="10"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="12"/>
       <c r="D23" s="3">
         <v>2</v>
       </c>
@@ -3314,14 +3342,14 @@
         <v>23</v>
       </c>
       <c r="G23" s="4"/>
-      <c r="H23" s="13"/>
+      <c r="H23" s="8"/>
       <c r="I23" s="6"/>
       <c r="J23" s="6"/>
     </row>
     <row r="24" spans="1:10" ht="21.75" thickBot="1">
       <c r="A24" s="6"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="10"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="12"/>
       <c r="D24" s="3">
         <v>3</v>
       </c>
@@ -3332,14 +3360,14 @@
         <v>19</v>
       </c>
       <c r="G24" s="4"/>
-      <c r="H24" s="13"/>
+      <c r="H24" s="8"/>
       <c r="I24" s="6"/>
       <c r="J24" s="6"/>
     </row>
     <row r="25" spans="1:10" ht="42.75" thickBot="1">
       <c r="A25" s="6"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="10"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="12"/>
       <c r="D25" s="3">
         <v>4</v>
       </c>
@@ -3350,14 +3378,14 @@
         <v>24</v>
       </c>
       <c r="G25" s="4"/>
-      <c r="H25" s="13"/>
+      <c r="H25" s="8"/>
       <c r="I25" s="6"/>
       <c r="J25" s="6"/>
     </row>
     <row r="26" spans="1:10" ht="84.75" thickBot="1">
       <c r="A26" s="6"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="10"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="12"/>
       <c r="D26" s="3">
         <v>5</v>
       </c>
@@ -3368,14 +3396,14 @@
         <v>98</v>
       </c>
       <c r="G26" s="4"/>
-      <c r="H26" s="13"/>
+      <c r="H26" s="8"/>
       <c r="I26" s="6"/>
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="21.75" thickBot="1">
       <c r="A27" s="6"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="10"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="12"/>
       <c r="D27" s="3">
         <v>6</v>
       </c>
@@ -3386,14 +3414,14 @@
         <v>108</v>
       </c>
       <c r="G27" s="4"/>
-      <c r="H27" s="13"/>
+      <c r="H27" s="8"/>
       <c r="I27" s="6"/>
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="32.25" thickBot="1">
       <c r="A28" s="6"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="10"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="12"/>
       <c r="D28" s="3">
         <v>7</v>
       </c>
@@ -3402,14 +3430,14 @@
       </c>
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
-      <c r="H28" s="13"/>
+      <c r="H28" s="8"/>
       <c r="I28" s="6"/>
       <c r="J28" s="6"/>
     </row>
     <row r="29" spans="1:10" ht="21.75" thickBot="1">
       <c r="A29" s="6"/>
-      <c r="B29" s="8"/>
-      <c r="C29" s="10"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="12"/>
       <c r="D29" s="3">
         <v>8</v>
       </c>
@@ -3420,14 +3448,14 @@
         <v>111</v>
       </c>
       <c r="G29" s="4"/>
-      <c r="H29" s="13"/>
+      <c r="H29" s="8"/>
       <c r="I29" s="6"/>
       <c r="J29" s="6"/>
     </row>
     <row r="30" spans="1:10" ht="32.25" thickBot="1">
       <c r="A30" s="6"/>
-      <c r="B30" s="8"/>
-      <c r="C30" s="10"/>
+      <c r="B30" s="10"/>
+      <c r="C30" s="12"/>
       <c r="D30" s="3">
         <v>9</v>
       </c>
@@ -3436,7 +3464,7 @@
       </c>
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
-      <c r="H30" s="13"/>
+      <c r="H30" s="8"/>
       <c r="I30" s="6"/>
       <c r="J30" s="6"/>
     </row>
@@ -3456,10 +3484,10 @@
       <c r="A32" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B32" s="7" t="s">
+      <c r="B32" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="C32" s="9" t="s">
+      <c r="C32" s="11" t="s">
         <v>113</v>
       </c>
       <c r="D32" s="3">
@@ -3472,7 +3500,7 @@
         <v>67</v>
       </c>
       <c r="G32" s="4"/>
-      <c r="H32" s="12" t="s">
+      <c r="H32" s="7" t="s">
         <v>9</v>
       </c>
       <c r="I32" s="5"/>
@@ -3480,8 +3508,8 @@
     </row>
     <row r="33" spans="1:10" ht="32.25" thickBot="1">
       <c r="A33" s="6"/>
-      <c r="B33" s="8"/>
-      <c r="C33" s="10"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="12"/>
       <c r="D33" s="3">
         <v>2</v>
       </c>
@@ -3492,14 +3520,14 @@
         <v>23</v>
       </c>
       <c r="G33" s="4"/>
-      <c r="H33" s="13"/>
+      <c r="H33" s="8"/>
       <c r="I33" s="6"/>
       <c r="J33" s="6"/>
     </row>
     <row r="34" spans="1:10" ht="21.75" thickBot="1">
       <c r="A34" s="6"/>
-      <c r="B34" s="8"/>
-      <c r="C34" s="10"/>
+      <c r="B34" s="10"/>
+      <c r="C34" s="12"/>
       <c r="D34" s="3">
         <v>3</v>
       </c>
@@ -3510,14 +3538,14 @@
         <v>19</v>
       </c>
       <c r="G34" s="4"/>
-      <c r="H34" s="13"/>
+      <c r="H34" s="8"/>
       <c r="I34" s="6"/>
       <c r="J34" s="6"/>
     </row>
     <row r="35" spans="1:10" ht="42.75" thickBot="1">
       <c r="A35" s="6"/>
-      <c r="B35" s="8"/>
-      <c r="C35" s="10"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="12"/>
       <c r="D35" s="3">
         <v>4</v>
       </c>
@@ -3528,14 +3556,14 @@
         <v>24</v>
       </c>
       <c r="G35" s="4"/>
-      <c r="H35" s="13"/>
+      <c r="H35" s="8"/>
       <c r="I35" s="6"/>
       <c r="J35" s="6"/>
     </row>
     <row r="36" spans="1:10" ht="84.75" thickBot="1">
       <c r="A36" s="6"/>
-      <c r="B36" s="8"/>
-      <c r="C36" s="10"/>
+      <c r="B36" s="10"/>
+      <c r="C36" s="12"/>
       <c r="D36" s="3">
         <v>5</v>
       </c>
@@ -3546,14 +3574,14 @@
         <v>98</v>
       </c>
       <c r="G36" s="4"/>
-      <c r="H36" s="13"/>
+      <c r="H36" s="8"/>
       <c r="I36" s="6"/>
       <c r="J36" s="6"/>
     </row>
     <row r="37" spans="1:10" ht="21.75" thickBot="1">
       <c r="A37" s="6"/>
-      <c r="B37" s="8"/>
-      <c r="C37" s="10"/>
+      <c r="B37" s="10"/>
+      <c r="C37" s="12"/>
       <c r="D37" s="3">
         <v>6</v>
       </c>
@@ -3564,14 +3592,14 @@
         <v>108</v>
       </c>
       <c r="G37" s="4"/>
-      <c r="H37" s="13"/>
+      <c r="H37" s="8"/>
       <c r="I37" s="6"/>
       <c r="J37" s="6"/>
     </row>
     <row r="38" spans="1:10" ht="32.25" thickBot="1">
       <c r="A38" s="6"/>
-      <c r="B38" s="8"/>
-      <c r="C38" s="10"/>
+      <c r="B38" s="10"/>
+      <c r="C38" s="12"/>
       <c r="D38" s="3">
         <v>7</v>
       </c>
@@ -3580,14 +3608,14 @@
       </c>
       <c r="F38" s="4"/>
       <c r="G38" s="4"/>
-      <c r="H38" s="13"/>
+      <c r="H38" s="8"/>
       <c r="I38" s="6"/>
       <c r="J38" s="6"/>
     </row>
     <row r="39" spans="1:10" ht="21.75" thickBot="1">
       <c r="A39" s="6"/>
-      <c r="B39" s="8"/>
-      <c r="C39" s="10"/>
+      <c r="B39" s="10"/>
+      <c r="C39" s="12"/>
       <c r="D39" s="3">
         <v>8</v>
       </c>
@@ -3598,14 +3626,14 @@
         <v>111</v>
       </c>
       <c r="G39" s="4"/>
-      <c r="H39" s="13"/>
+      <c r="H39" s="8"/>
       <c r="I39" s="6"/>
       <c r="J39" s="6"/>
     </row>
     <row r="40" spans="1:10" ht="32.25" thickBot="1">
       <c r="A40" s="6"/>
-      <c r="B40" s="8"/>
-      <c r="C40" s="10"/>
+      <c r="B40" s="10"/>
+      <c r="C40" s="12"/>
       <c r="D40" s="3">
         <v>9</v>
       </c>
@@ -3614,14 +3642,14 @@
       </c>
       <c r="F40" s="4"/>
       <c r="G40" s="4"/>
-      <c r="H40" s="13"/>
+      <c r="H40" s="8"/>
       <c r="I40" s="6"/>
       <c r="J40" s="6"/>
     </row>
     <row r="41" spans="1:10" ht="42.75" thickBot="1">
       <c r="A41" s="6"/>
-      <c r="B41" s="8"/>
-      <c r="C41" s="10"/>
+      <c r="B41" s="10"/>
+      <c r="C41" s="12"/>
       <c r="D41" s="3">
         <v>10</v>
       </c>
@@ -3632,7 +3660,7 @@
         <v>117</v>
       </c>
       <c r="G41" s="4"/>
-      <c r="H41" s="13"/>
+      <c r="H41" s="8"/>
       <c r="I41" s="6"/>
       <c r="J41" s="6"/>
     </row>
@@ -3650,6 +3678,18 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="I2:I9"/>
+    <mergeCell ref="J2:J9"/>
+    <mergeCell ref="A11:A20"/>
+    <mergeCell ref="B11:B20"/>
+    <mergeCell ref="C11:C20"/>
+    <mergeCell ref="H11:H20"/>
+    <mergeCell ref="I11:I20"/>
+    <mergeCell ref="J11:J20"/>
+    <mergeCell ref="A2:A9"/>
+    <mergeCell ref="B2:B9"/>
+    <mergeCell ref="C2:C9"/>
+    <mergeCell ref="H2:H9"/>
     <mergeCell ref="J22:J30"/>
     <mergeCell ref="A32:A41"/>
     <mergeCell ref="B32:B41"/>
@@ -3662,18 +3702,6 @@
     <mergeCell ref="C22:C30"/>
     <mergeCell ref="H22:H30"/>
     <mergeCell ref="I22:I30"/>
-    <mergeCell ref="I2:I9"/>
-    <mergeCell ref="J2:J9"/>
-    <mergeCell ref="A11:A20"/>
-    <mergeCell ref="B11:B20"/>
-    <mergeCell ref="C11:C20"/>
-    <mergeCell ref="H11:H20"/>
-    <mergeCell ref="I11:I20"/>
-    <mergeCell ref="J11:J20"/>
-    <mergeCell ref="A2:A9"/>
-    <mergeCell ref="B2:B9"/>
-    <mergeCell ref="C2:C9"/>
-    <mergeCell ref="H2:H9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -3700,13 +3728,19 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="17.28515625" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" customWidth="1"/>
+    <col min="5" max="5" width="25" customWidth="1"/>
+    <col min="6" max="6" width="26.140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="21.75" thickBot="1">
       <c r="A1" s="1" t="s">
@@ -3740,101 +3774,101 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="63.75" thickBot="1">
+    <row r="2" spans="1:10" ht="21.75" thickBot="1">
       <c r="A2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="11" t="s">
         <v>45</v>
       </c>
       <c r="D2" s="3">
         <v>1</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>22</v>
+        <v>81</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>23</v>
+        <v>67</v>
       </c>
       <c r="G2" s="4"/>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="7" t="s">
         <v>9</v>
       </c>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
     </row>
-    <row r="3" spans="1:10" ht="42.75" thickBot="1">
+    <row r="3" spans="1:10" ht="21.75" thickBot="1">
       <c r="A3" s="6"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="10"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="12"/>
       <c r="D3" s="3">
         <v>2</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>18</v>
+      <c r="E3" s="14" t="s">
+        <v>123</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>19</v>
       </c>
       <c r="G3" s="4"/>
-      <c r="H3" s="13"/>
+      <c r="H3" s="8"/>
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
     </row>
-    <row r="4" spans="1:10" ht="105.75" thickBot="1">
+    <row r="4" spans="1:10" ht="21.75" thickBot="1">
       <c r="A4" s="6"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="10"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="12"/>
       <c r="D4" s="3">
         <v>3</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="G4" s="4"/>
-      <c r="H4" s="13"/>
+      <c r="H4" s="8"/>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
     </row>
-    <row r="5" spans="1:10" ht="74.25" thickBot="1">
+    <row r="5" spans="1:10" ht="32.25" thickBot="1">
       <c r="A5" s="6"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="10"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="12"/>
       <c r="D5" s="3">
         <v>4</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>48</v>
+        <v>124</v>
       </c>
       <c r="G5" s="4"/>
-      <c r="H5" s="13"/>
+      <c r="H5" s="8"/>
       <c r="I5" s="6"/>
       <c r="J5" s="6"/>
     </row>
-    <row r="6" spans="1:10" ht="74.25" thickBot="1">
+    <row r="6" spans="1:10" ht="32.25" thickBot="1">
       <c r="A6" s="6"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="10"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="12"/>
       <c r="D6" s="3">
         <v>5</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>49</v>
+        <v>125</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>50</v>
+        <v>126</v>
       </c>
       <c r="G6" s="4"/>
-      <c r="H6" s="13"/>
+      <c r="H6" s="8"/>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
     </row>
@@ -3850,132 +3884,17 @@
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
     </row>
-    <row r="8" spans="1:10" ht="63.75" thickBot="1">
-      <c r="A8" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="D8" s="3">
-        <v>1</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G8" s="4"/>
-      <c r="H8" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-    </row>
-    <row r="9" spans="1:10" ht="42.75" thickBot="1">
-      <c r="A9" s="6"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="3">
-        <v>2</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G9" s="4"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-    </row>
-    <row r="10" spans="1:10" ht="105.75" thickBot="1">
-      <c r="A10" s="6"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="3">
-        <v>3</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G10" s="4"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-    </row>
-    <row r="11" spans="1:10" ht="74.25" thickBot="1">
-      <c r="A11" s="6"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="3">
-        <v>4</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="G11" s="4"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-    </row>
-    <row r="12" spans="1:10" ht="95.25" thickBot="1">
-      <c r="A12" s="6"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="3">
-        <v>5</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="G12" s="4"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-    </row>
-    <row r="13" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-    </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="6">
     <mergeCell ref="I2:I6"/>
     <mergeCell ref="J2:J6"/>
-    <mergeCell ref="A8:A12"/>
-    <mergeCell ref="B8:B12"/>
-    <mergeCell ref="C8:C12"/>
-    <mergeCell ref="H8:H12"/>
-    <mergeCell ref="I8:I12"/>
-    <mergeCell ref="J8:J12"/>
     <mergeCell ref="A2:A6"/>
     <mergeCell ref="B2:B6"/>
     <mergeCell ref="C2:C6"/>
     <mergeCell ref="H2:H6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
@@ -3983,13 +3902,13 @@
           <x14:formula1>
             <xm:f>Reference!$C$1:$C$4</xm:f>
           </x14:formula1>
-          <xm:sqref>I2:I6 I8:I12</xm:sqref>
+          <xm:sqref>I2:I6</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Reference!$A$1:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>H2:H6 H8:H12</xm:sqref>
+          <xm:sqref>H2:H6</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -4001,7 +3920,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8:C12"/>
     </sheetView>
   </sheetViews>
@@ -4043,10 +3962,10 @@
       <c r="A2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="11" t="s">
         <v>45</v>
       </c>
       <c r="D2" s="3">
@@ -4059,7 +3978,7 @@
         <v>23</v>
       </c>
       <c r="G2" s="4"/>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="7" t="s">
         <v>9</v>
       </c>
       <c r="I2" s="5"/>
@@ -4067,8 +3986,8 @@
     </row>
     <row r="3" spans="1:10" ht="42.75" thickBot="1">
       <c r="A3" s="6"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="10"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="12"/>
       <c r="D3" s="3">
         <v>2</v>
       </c>
@@ -4079,14 +3998,14 @@
         <v>19</v>
       </c>
       <c r="G3" s="4"/>
-      <c r="H3" s="13"/>
+      <c r="H3" s="8"/>
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
     </row>
     <row r="4" spans="1:10" ht="105.75" thickBot="1">
       <c r="A4" s="6"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="10"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="12"/>
       <c r="D4" s="3">
         <v>3</v>
       </c>
@@ -4097,14 +4016,14 @@
         <v>24</v>
       </c>
       <c r="G4" s="4"/>
-      <c r="H4" s="13"/>
+      <c r="H4" s="8"/>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
     </row>
     <row r="5" spans="1:10" ht="74.25" thickBot="1">
       <c r="A5" s="6"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="10"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="12"/>
       <c r="D5" s="3">
         <v>4</v>
       </c>
@@ -4115,14 +4034,14 @@
         <v>48</v>
       </c>
       <c r="G5" s="4"/>
-      <c r="H5" s="13"/>
+      <c r="H5" s="8"/>
       <c r="I5" s="6"/>
       <c r="J5" s="6"/>
     </row>
     <row r="6" spans="1:10" ht="74.25" thickBot="1">
       <c r="A6" s="6"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="10"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="12"/>
       <c r="D6" s="3">
         <v>5</v>
       </c>
@@ -4133,7 +4052,7 @@
         <v>50</v>
       </c>
       <c r="G6" s="4"/>
-      <c r="H6" s="13"/>
+      <c r="H6" s="8"/>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
     </row>
@@ -4153,10 +4072,10 @@
       <c r="A8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="11" t="s">
         <v>52</v>
       </c>
       <c r="D8" s="3">
@@ -4169,7 +4088,7 @@
         <v>23</v>
       </c>
       <c r="G8" s="4"/>
-      <c r="H8" s="12" t="s">
+      <c r="H8" s="7" t="s">
         <v>9</v>
       </c>
       <c r="I8" s="5"/>
@@ -4177,8 +4096,8 @@
     </row>
     <row r="9" spans="1:10" ht="42.75" thickBot="1">
       <c r="A9" s="6"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="10"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="12"/>
       <c r="D9" s="3">
         <v>2</v>
       </c>
@@ -4189,14 +4108,14 @@
         <v>19</v>
       </c>
       <c r="G9" s="4"/>
-      <c r="H9" s="13"/>
+      <c r="H9" s="8"/>
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
     </row>
     <row r="10" spans="1:10" ht="105.75" thickBot="1">
       <c r="A10" s="6"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="10"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="12"/>
       <c r="D10" s="3">
         <v>3</v>
       </c>
@@ -4207,14 +4126,14 @@
         <v>24</v>
       </c>
       <c r="G10" s="4"/>
-      <c r="H10" s="13"/>
+      <c r="H10" s="8"/>
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
     </row>
     <row r="11" spans="1:10" ht="74.25" thickBot="1">
       <c r="A11" s="6"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="10"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="12"/>
       <c r="D11" s="3">
         <v>4</v>
       </c>
@@ -4225,14 +4144,14 @@
         <v>48</v>
       </c>
       <c r="G11" s="4"/>
-      <c r="H11" s="13"/>
+      <c r="H11" s="8"/>
       <c r="I11" s="6"/>
       <c r="J11" s="6"/>
     </row>
     <row r="12" spans="1:10" ht="95.25" thickBot="1">
       <c r="A12" s="6"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="10"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="12"/>
       <c r="D12" s="3">
         <v>5</v>
       </c>
@@ -4243,7 +4162,7 @@
         <v>54</v>
       </c>
       <c r="G12" s="4"/>
-      <c r="H12" s="13"/>
+      <c r="H12" s="8"/>
       <c r="I12" s="6"/>
       <c r="J12" s="6"/>
     </row>

</xml_diff>

<commit_message>
US 7 no puede ser testeada
</commit_message>
<xml_diff>
--- a/Docs/08-Prueba/Tests Cases - Modulo de Planificación.xlsx
+++ b/Docs/08-Prueba/Tests Cases - Modulo de Planificación.xlsx
@@ -13,7 +13,6 @@
     <sheet name="US_1" sheetId="30" r:id="rId4"/>
     <sheet name="US_2" sheetId="31" r:id="rId5"/>
     <sheet name="US_3" sheetId="32" r:id="rId6"/>
-    <sheet name="US_7" sheetId="34" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">US_135!$A$1:$J$1</definedName>
@@ -23,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="126">
   <si>
     <t>Application</t>
   </si>
@@ -157,9 +156,6 @@
     <t>El sistema muestra una advertencia indicando que la descripción es requerido.</t>
   </si>
   <si>
-    <t>TC1_US7</t>
-  </si>
-  <si>
     <t>Este Test Case tiene como objeto verificar la eliminación satisfactoria de un contenido.</t>
   </si>
   <si>
@@ -176,9 +172,6 @@
   </si>
   <si>
     <t>El sistema elimina el contenido seleccionado, este ya no es mostrado en el listado.</t>
-  </si>
-  <si>
-    <t>TC2_US7</t>
   </si>
   <si>
     <t>Este Test Case tiene como objeto verificar que la eliminación de un contenido no es llevada a cabo si el usuario no confirma la operación.</t>
@@ -472,6 +465,9 @@
   </si>
   <si>
     <t>El sistema despliega el plan de la misma</t>
+  </si>
+  <si>
+    <t>Este Test Case tiene como objeto verificar que el usuario puede realizar una consulta sobre un determinado plan.</t>
   </si>
 </sst>
 </file>
@@ -1057,7 +1053,7 @@
         <v>8</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C2" s="11" t="s">
         <v>21</v>
@@ -1066,10 +1062,10 @@
         <v>1</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G2" s="4"/>
       <c r="H2" s="7"/>
@@ -1138,7 +1134,7 @@
         <v>5</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>25</v>
@@ -1183,7 +1179,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>29</v>
@@ -1192,10 +1188,10 @@
         <v>1</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G9" s="4"/>
       <c r="H9" s="7"/>
@@ -1309,7 +1305,7 @@
         <v>8</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C16" s="11" t="s">
         <v>32</v>
@@ -1318,10 +1314,10 @@
         <v>1</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G16" s="4"/>
       <c r="H16" s="7"/>
@@ -1453,7 +1449,7 @@
         <v>8</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C24" s="11" t="s">
         <v>40</v>
@@ -1462,10 +1458,10 @@
         <v>1</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G24" s="4"/>
       <c r="H24" s="7"/>
@@ -1579,7 +1575,7 @@
         <v>8</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C31" s="11" t="s">
         <v>41</v>
@@ -1588,10 +1584,10 @@
         <v>1</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G31" s="4"/>
       <c r="H31" s="7"/>
@@ -1827,19 +1823,19 @@
         <v>8</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D2" s="3">
         <v>1</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G2" s="4"/>
       <c r="H2" s="7" t="s">
@@ -1910,10 +1906,10 @@
         <v>5</v>
       </c>
       <c r="E6" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>47</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>48</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="8"/>
@@ -1928,10 +1924,10 @@
         <v>6</v>
       </c>
       <c r="E7" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F7" s="4" t="s">
         <v>49</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>50</v>
       </c>
       <c r="G7" s="4"/>
       <c r="H7" s="8"/>
@@ -1955,19 +1951,19 @@
         <v>8</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D9" s="3">
         <v>1</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G9" s="4"/>
       <c r="H9" s="7" t="s">
@@ -2038,10 +2034,10 @@
         <v>5</v>
       </c>
       <c r="E13" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" s="4" t="s">
         <v>47</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>48</v>
       </c>
       <c r="G13" s="4"/>
       <c r="H13" s="8"/>
@@ -2056,10 +2052,10 @@
         <v>6</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G14" s="4"/>
       <c r="H14" s="8"/>
@@ -2169,19 +2165,19 @@
         <v>8</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D2" s="3">
         <v>1</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G2" s="4"/>
       <c r="H2" s="7" t="s">
@@ -2198,10 +2194,10 @@
         <v>2</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G3" s="4"/>
       <c r="H3" s="8"/>
@@ -2234,10 +2230,10 @@
         <v>4</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G5" s="4"/>
       <c r="H5" s="8"/>
@@ -2252,10 +2248,10 @@
         <v>5</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="8"/>
@@ -2279,19 +2275,19 @@
         <v>8</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D8" s="3">
         <v>1</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G8" s="4"/>
       <c r="H8" s="7" t="s">
@@ -2326,7 +2322,7 @@
         <v>3</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>19</v>
@@ -2344,10 +2340,10 @@
         <v>4</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="8"/>
@@ -2371,19 +2367,19 @@
         <v>8</v>
       </c>
       <c r="B13" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C13" s="11" t="s">
         <v>77</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>79</v>
       </c>
       <c r="D13" s="3">
         <v>1</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G13" s="4"/>
       <c r="H13" s="7" t="s">
@@ -2400,10 +2396,10 @@
         <v>2</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G14" s="4"/>
       <c r="H14" s="8"/>
@@ -2439,7 +2435,7 @@
         <v>20</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G16" s="4"/>
       <c r="H16" s="8"/>
@@ -2463,19 +2459,19 @@
         <v>8</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D18" s="3">
         <v>1</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G18" s="4"/>
       <c r="H18" s="7" t="s">
@@ -2492,10 +2488,10 @@
         <v>2</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G19" s="4"/>
       <c r="H19" s="8"/>
@@ -2528,10 +2524,10 @@
         <v>4</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G21" s="4"/>
       <c r="H21" s="8"/>
@@ -2546,10 +2542,10 @@
         <v>5</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G22" s="4"/>
       <c r="H22" s="8"/>
@@ -2564,10 +2560,10 @@
         <v>6</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G23" s="4"/>
       <c r="H23" s="8"/>
@@ -2582,7 +2578,7 @@
         <v>7</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
@@ -2598,7 +2594,7 @@
         <v>8</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
@@ -2614,7 +2610,7 @@
         <v>9</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
@@ -2630,10 +2626,10 @@
         <v>10</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G27" s="4"/>
       <c r="H27" s="8"/>
@@ -2657,19 +2653,19 @@
         <v>8</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D29" s="3">
         <v>1</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G29" s="4"/>
       <c r="H29" s="7" t="s">
@@ -2686,10 +2682,10 @@
         <v>2</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G30" s="4"/>
       <c r="H30" s="8"/>
@@ -2722,10 +2718,10 @@
         <v>4</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G32" s="4"/>
       <c r="H32" s="8"/>
@@ -2740,10 +2736,10 @@
         <v>5</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G33" s="4"/>
       <c r="H33" s="8"/>
@@ -2758,10 +2754,10 @@
         <v>6</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G34" s="4"/>
       <c r="H34" s="8"/>
@@ -2776,10 +2772,10 @@
         <v>7</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G35" s="4"/>
       <c r="H35" s="8"/>
@@ -2794,7 +2790,7 @@
         <v>8</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F36" s="4"/>
       <c r="G36" s="4"/>
@@ -2810,7 +2806,7 @@
         <v>9</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F37" s="4"/>
       <c r="G37" s="4"/>
@@ -2826,10 +2822,10 @@
         <v>10</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G38" s="4"/>
       <c r="H38" s="8"/>
@@ -2908,7 +2904,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
@@ -2955,19 +2951,19 @@
         <v>8</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D2" s="3">
         <v>1</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G2" s="4"/>
       <c r="H2" s="7" t="s">
@@ -3038,10 +3034,10 @@
         <v>5</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="8"/>
@@ -3056,7 +3052,7 @@
         <v>6</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
@@ -3072,7 +3068,7 @@
         <v>7</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
@@ -3088,7 +3084,7 @@
         <v>8</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
@@ -3113,19 +3109,19 @@
         <v>8</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D11" s="3">
         <v>1</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="7" t="s">
@@ -3196,10 +3192,10 @@
         <v>5</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G15" s="4"/>
       <c r="H15" s="8"/>
@@ -3214,7 +3210,7 @@
         <v>6</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
@@ -3230,7 +3226,7 @@
         <v>7</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
@@ -3246,7 +3242,7 @@
         <v>8</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
@@ -3262,10 +3258,10 @@
         <v>9</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G19" s="4"/>
       <c r="H19" s="8"/>
@@ -3280,10 +3276,10 @@
         <v>10</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G20" s="4"/>
       <c r="H20" s="8"/>
@@ -3307,19 +3303,19 @@
         <v>8</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D22" s="3">
         <v>1</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G22" s="4"/>
       <c r="H22" s="7" t="s">
@@ -3390,10 +3386,10 @@
         <v>5</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G26" s="4"/>
       <c r="H26" s="8"/>
@@ -3408,10 +3404,10 @@
         <v>6</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G27" s="4"/>
       <c r="H27" s="8"/>
@@ -3426,7 +3422,7 @@
         <v>7</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
@@ -3442,10 +3438,10 @@
         <v>8</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G29" s="4"/>
       <c r="H29" s="8"/>
@@ -3460,7 +3456,7 @@
         <v>9</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
@@ -3485,19 +3481,19 @@
         <v>8</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D32" s="3">
         <v>1</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G32" s="4"/>
       <c r="H32" s="7" t="s">
@@ -3568,10 +3564,10 @@
         <v>5</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G36" s="4"/>
       <c r="H36" s="8"/>
@@ -3586,10 +3582,10 @@
         <v>6</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G37" s="4"/>
       <c r="H37" s="8"/>
@@ -3604,7 +3600,7 @@
         <v>7</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F38" s="4"/>
       <c r="G38" s="4"/>
@@ -3620,10 +3616,10 @@
         <v>8</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G39" s="4"/>
       <c r="H39" s="8"/>
@@ -3638,7 +3634,7 @@
         <v>9</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F40" s="4"/>
       <c r="G40" s="4"/>
@@ -3654,10 +3650,10 @@
         <v>10</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="G41" s="4"/>
       <c r="H41" s="8"/>
@@ -3731,7 +3727,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C2" sqref="C2:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3779,19 +3775,19 @@
         <v>8</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>45</v>
+        <v>125</v>
       </c>
       <c r="D2" s="3">
         <v>1</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G2" s="4"/>
       <c r="H2" s="7" t="s">
@@ -3808,7 +3804,7 @@
         <v>2</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>19</v>
@@ -3844,10 +3840,10 @@
         <v>4</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="G5" s="4"/>
       <c r="H5" s="8"/>
@@ -3862,10 +3858,10 @@
         <v>5</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="8"/>
@@ -3914,303 +3910,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8:C12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:10" ht="21.75" thickBot="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="63.75" thickBot="1">
-      <c r="A2" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="D2" s="3">
-        <v>1</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" s="4"/>
-      <c r="H2" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-    </row>
-    <row r="3" spans="1:10" ht="42.75" thickBot="1">
-      <c r="A3" s="6"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="3">
-        <v>2</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="4"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-    </row>
-    <row r="4" spans="1:10" ht="105.75" thickBot="1">
-      <c r="A4" s="6"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="3">
-        <v>3</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4" s="4"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-    </row>
-    <row r="5" spans="1:10" ht="74.25" thickBot="1">
-      <c r="A5" s="6"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="3">
-        <v>4</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="G5" s="4"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-    </row>
-    <row r="6" spans="1:10" ht="74.25" thickBot="1">
-      <c r="A6" s="6"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="3">
-        <v>5</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="G6" s="4"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-    </row>
-    <row r="7" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-    </row>
-    <row r="8" spans="1:10" ht="63.75" thickBot="1">
-      <c r="A8" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="D8" s="3">
-        <v>1</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G8" s="4"/>
-      <c r="H8" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-    </row>
-    <row r="9" spans="1:10" ht="42.75" thickBot="1">
-      <c r="A9" s="6"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="3">
-        <v>2</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G9" s="4"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-    </row>
-    <row r="10" spans="1:10" ht="105.75" thickBot="1">
-      <c r="A10" s="6"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="3">
-        <v>3</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G10" s="4"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-    </row>
-    <row r="11" spans="1:10" ht="74.25" thickBot="1">
-      <c r="A11" s="6"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="3">
-        <v>4</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="G11" s="4"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-    </row>
-    <row r="12" spans="1:10" ht="95.25" thickBot="1">
-      <c r="A12" s="6"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="3">
-        <v>5</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="G12" s="4"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-    </row>
-    <row r="13" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-    </row>
-  </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="J8:J12"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="B2:B6"/>
-    <mergeCell ref="C2:C6"/>
-    <mergeCell ref="H2:H6"/>
-    <mergeCell ref="I2:I6"/>
-    <mergeCell ref="J2:J6"/>
-    <mergeCell ref="A8:A12"/>
-    <mergeCell ref="B8:B12"/>
-    <mergeCell ref="C8:C12"/>
-    <mergeCell ref="H8:H12"/>
-    <mergeCell ref="I8:I12"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Reference!$C$1:$C$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>I2:I6 I8:I12</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Reference!$A$1:$A$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>H2:H6 H8:H12</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
 </file>
</xml_diff>